<commit_message>
added notes for b1.d1
</commit_message>
<xml_diff>
--- a/data/curve_data/ldeli_tinc_integrate.xlsx
+++ b/data/curve_data/ldeli_tinc_integrate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fontikar/Dropbox/Ldeli_inc_metabTelo/data/curve_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99C0BA1E-4268-F04D-AC3F-6F96F3B1A239}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAE22156-4FA1-684F-A3B6-7508E6A9D331}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="1800" windowWidth="31740" windowHeight="16940" xr2:uid="{84C113A7-A3A6-0745-8C21-C9F341A27D93}"/>
+    <workbookView xWindow="1980" yWindow="1800" windowWidth="36360" windowHeight="16940" xr2:uid="{84C113A7-A3A6-0745-8C21-C9F341A27D93}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="85">
   <si>
     <t>date</t>
   </si>
@@ -81,9 +81,6 @@
     <t>defecate</t>
   </si>
   <si>
-    <t>air_collect_notes</t>
-  </si>
-  <si>
     <t>fms_notes</t>
   </si>
   <si>
@@ -174,7 +171,115 @@
     <t>lizmass</t>
   </si>
   <si>
-    <t>test</t>
+    <t>key</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>processed D before C</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>SH</t>
+  </si>
+  <si>
+    <t>CH</t>
+  </si>
+  <si>
+    <t>1CR, SH</t>
+  </si>
+  <si>
+    <t>WB</t>
+  </si>
+  <si>
+    <t>6 instead of F</t>
+  </si>
+  <si>
+    <t>T2CL</t>
+  </si>
+  <si>
+    <t>NPT2S</t>
+  </si>
+  <si>
+    <t>T2CFS,L</t>
+  </si>
+  <si>
+    <t>T1S1L</t>
   </si>
 </sst>
 </file>
@@ -309,7 +414,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -359,6 +464,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Accent3" xfId="1" builtinId="38"/>
@@ -674,11 +783,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40F86C92-9F04-9A44-AFB8-57BF91CE8886}">
-  <dimension ref="A1:X101"/>
+  <dimension ref="A1:Y101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q2" sqref="Q2:Q5"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W27" sqref="W27:X51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -690,12 +799,12 @@
     <col min="9" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="17" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" s="17" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C1" s="17" t="s">
         <v>1</v>
@@ -710,7 +819,7 @@
         <v>2</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H1" s="17" t="s">
         <v>4</v>
@@ -728,7 +837,7 @@
         <v>9</v>
       </c>
       <c r="M1" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N1" s="19" t="s">
         <v>10</v>
@@ -739,7 +848,7 @@
       <c r="P1" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="20" t="s">
+      <c r="Q1" s="23" t="s">
         <v>13</v>
       </c>
       <c r="R1" s="21" t="s">
@@ -751,20 +860,23 @@
       <c r="T1" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="17" t="s">
+      <c r="U1" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="V1" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="V1" s="22" t="s">
+      <c r="W1" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="X1" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="W1" s="17" t="s">
+      <c r="Y1" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="X1" s="17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:25" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>43197</v>
       </c>
@@ -778,7 +890,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F2" s="5">
         <v>1</v>
@@ -815,11 +927,15 @@
         <f>TEXT(O2-N2, "[mm]")</f>
         <v>132</v>
       </c>
-      <c r="Q2" s="11" t="s">
+      <c r="Q2" s="3"/>
+      <c r="U2" s="11" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="V2" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>43197</v>
       </c>
@@ -833,7 +949,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F3" s="1">
         <v>2</v>
@@ -870,11 +986,17 @@
         <f t="shared" ref="P3:P66" si="1">TEXT(O3-N3, "[mm]")</f>
         <v>132</v>
       </c>
-      <c r="Q3" s="11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="U3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="V3" s="3">
+        <v>0</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>43197</v>
       </c>
@@ -888,7 +1010,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4" s="1">
         <v>3</v>
@@ -925,11 +1047,17 @@
         <f t="shared" si="1"/>
         <v>132</v>
       </c>
-      <c r="Q4" s="11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="U4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="V4" s="3">
+        <v>1</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>43197</v>
       </c>
@@ -943,7 +1071,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F5" s="1">
         <v>4</v>
@@ -980,11 +1108,14 @@
         <f t="shared" si="1"/>
         <v>132</v>
       </c>
-      <c r="Q5" s="11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="U5" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="V5" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>43197</v>
       </c>
@@ -998,7 +1129,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F6" s="1">
         <v>5</v>
@@ -1035,8 +1166,14 @@
         <f t="shared" si="1"/>
         <v>132</v>
       </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="U6" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="V6" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <v>43197</v>
       </c>
@@ -1050,7 +1187,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F7" s="1">
         <v>6</v>
@@ -1087,8 +1224,20 @@
         <f t="shared" si="1"/>
         <v>132</v>
       </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="U7" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="V7" s="24">
+        <v>0</v>
+      </c>
+      <c r="W7" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="X7" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>43197</v>
       </c>
@@ -1102,7 +1251,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F8" s="1">
         <v>7</v>
@@ -1139,8 +1288,20 @@
         <f t="shared" si="1"/>
         <v>132</v>
       </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="U8" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="V8" s="24">
+        <v>1</v>
+      </c>
+      <c r="W8" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="X8" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <v>43197</v>
       </c>
@@ -1154,7 +1315,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F9" s="1">
         <v>8</v>
@@ -1191,8 +1352,14 @@
         <f t="shared" si="1"/>
         <v>132</v>
       </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="U9" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="V9" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <v>43197</v>
       </c>
@@ -1206,7 +1373,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F10" s="1">
         <v>9</v>
@@ -1243,8 +1410,17 @@
         <f t="shared" si="1"/>
         <v>132</v>
       </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="U10" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="V10" s="24">
+        <v>1</v>
+      </c>
+      <c r="W10" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
         <v>43197</v>
       </c>
@@ -1258,7 +1434,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F11" s="1">
         <v>10</v>
@@ -1295,8 +1471,17 @@
         <f t="shared" si="1"/>
         <v>132</v>
       </c>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="U11" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="V11" s="24">
+        <v>1</v>
+      </c>
+      <c r="W11" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
         <v>43197</v>
       </c>
@@ -1310,7 +1495,7 @@
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F12" s="1">
         <v>11</v>
@@ -1347,8 +1532,17 @@
         <f t="shared" si="1"/>
         <v>132</v>
       </c>
-    </row>
-    <row r="13" spans="1:24" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U12" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="V12" s="24">
+        <v>1</v>
+      </c>
+      <c r="W12" s="24" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8">
         <v>43197</v>
       </c>
@@ -1362,7 +1556,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F13" s="9">
         <v>12</v>
@@ -1399,8 +1593,14 @@
         <f t="shared" si="1"/>
         <v>132</v>
       </c>
-    </row>
-    <row r="14" spans="1:24" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U13" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="V13" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>43197</v>
       </c>
@@ -1414,7 +1614,7 @@
         <v>2</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F14" s="5">
         <v>13</v>
@@ -1451,8 +1651,14 @@
         <f t="shared" si="1"/>
         <v>193</v>
       </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="U14" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="V14" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
         <v>43197</v>
       </c>
@@ -1466,7 +1672,7 @@
         <v>2</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F15" s="1">
         <v>14</v>
@@ -1503,8 +1709,20 @@
         <f t="shared" si="1"/>
         <v>193</v>
       </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="U15" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="V15" s="24">
+        <v>1</v>
+      </c>
+      <c r="W15" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="X15" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
         <v>43197</v>
       </c>
@@ -1518,7 +1736,7 @@
         <v>2</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F16" s="1">
         <v>15</v>
@@ -1555,8 +1773,14 @@
         <f t="shared" si="1"/>
         <v>193</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="U16" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="V16" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
         <v>43197</v>
       </c>
@@ -1570,7 +1794,7 @@
         <v>2</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F17" s="1">
         <v>16</v>
@@ -1607,8 +1831,14 @@
         <f t="shared" si="1"/>
         <v>193</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="U17" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="V17" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
         <v>43197</v>
       </c>
@@ -1622,7 +1852,7 @@
         <v>2</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F18" s="1">
         <v>17</v>
@@ -1659,8 +1889,14 @@
         <f t="shared" si="1"/>
         <v>193</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="U18" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="V18" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A19" s="7">
         <v>43197</v>
       </c>
@@ -1674,7 +1910,7 @@
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F19" s="1">
         <v>18</v>
@@ -1711,8 +1947,17 @@
         <f t="shared" si="1"/>
         <v>193</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="U19" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="V19" s="24">
+        <v>0</v>
+      </c>
+      <c r="X19" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20" s="7">
         <v>43197</v>
       </c>
@@ -1726,7 +1971,7 @@
         <v>2</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F20" s="1">
         <v>19</v>
@@ -1763,8 +2008,14 @@
         <f t="shared" si="1"/>
         <v>193</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="U20" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="V20" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21" s="7">
         <v>43197</v>
       </c>
@@ -1778,7 +2029,7 @@
         <v>2</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F21" s="1">
         <v>20</v>
@@ -1815,8 +2066,17 @@
         <f t="shared" si="1"/>
         <v>193</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="U21" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="V21" s="24">
+        <v>1</v>
+      </c>
+      <c r="W21" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A22" s="7">
         <v>43197</v>
       </c>
@@ -1830,7 +2090,7 @@
         <v>2</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F22" s="1">
         <v>21</v>
@@ -1867,8 +2127,14 @@
         <f t="shared" si="1"/>
         <v>193</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="U22" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="V22" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A23" s="7">
         <v>43197</v>
       </c>
@@ -1882,7 +2148,7 @@
         <v>2</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F23" s="1">
         <v>22</v>
@@ -1919,8 +2185,14 @@
         <f t="shared" si="1"/>
         <v>193</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="U23" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="V23" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24" s="7">
         <v>43197</v>
       </c>
@@ -1934,7 +2206,7 @@
         <v>2</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F24" s="1">
         <v>23</v>
@@ -1971,8 +2243,14 @@
         <f t="shared" si="1"/>
         <v>193</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="U24" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="V24" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A25" s="7">
         <v>43197</v>
       </c>
@@ -1986,7 +2264,7 @@
         <v>2</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F25" s="1">
         <v>24</v>
@@ -2023,8 +2301,14 @@
         <f t="shared" si="1"/>
         <v>193</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U25" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="V25" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="8">
         <v>43197</v>
       </c>
@@ -2038,7 +2322,7 @@
         <v>2</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F26" s="9">
         <v>25</v>
@@ -2075,8 +2359,14 @@
         <f t="shared" si="1"/>
         <v>193</v>
       </c>
-    </row>
-    <row r="27" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U26" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="V26" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
         <v>43197</v>
       </c>
@@ -2090,7 +2380,7 @@
         <v>1</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F27" s="5">
         <v>1</v>
@@ -2127,8 +2417,14 @@
         <f t="shared" si="1"/>
         <v>192</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="U27" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="V27" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A28" s="7">
         <v>43197</v>
       </c>
@@ -2142,7 +2438,7 @@
         <v>1</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F28" s="1">
         <v>2</v>
@@ -2179,8 +2475,17 @@
         <f t="shared" si="1"/>
         <v>192</v>
       </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="U28" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="V28" s="3">
+        <v>0</v>
+      </c>
+      <c r="W28" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A29" s="7">
         <v>43197</v>
       </c>
@@ -2194,7 +2499,7 @@
         <v>1</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F29" s="1">
         <v>3</v>
@@ -2231,8 +2536,17 @@
         <f t="shared" si="1"/>
         <v>192</v>
       </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="U29" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="V29" s="3">
+        <v>1</v>
+      </c>
+      <c r="X29" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A30" s="7">
         <v>43197</v>
       </c>
@@ -2246,7 +2560,7 @@
         <v>1</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F30" s="1">
         <v>4</v>
@@ -2283,8 +2597,14 @@
         <f t="shared" si="1"/>
         <v>192</v>
       </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="U30" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="V30" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A31" s="7">
         <v>43197</v>
       </c>
@@ -2298,7 +2618,7 @@
         <v>1</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F31" s="1">
         <v>5</v>
@@ -2335,8 +2655,14 @@
         <f t="shared" si="1"/>
         <v>192</v>
       </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="U31" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="V31" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A32" s="7">
         <v>43197</v>
       </c>
@@ -2350,7 +2676,7 @@
         <v>1</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F32" s="1">
         <v>6</v>
@@ -2387,8 +2713,20 @@
         <f t="shared" si="1"/>
         <v>192</v>
       </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="U32" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="V32" s="24">
+        <v>0</v>
+      </c>
+      <c r="W32" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="X32" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A33" s="7">
         <v>43197</v>
       </c>
@@ -2402,7 +2740,7 @@
         <v>1</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F33" s="1">
         <v>7</v>
@@ -2439,8 +2777,20 @@
         <f t="shared" si="1"/>
         <v>192</v>
       </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="U33" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="V33" s="24">
+        <v>1</v>
+      </c>
+      <c r="W33" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="X33" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A34" s="7">
         <v>43197</v>
       </c>
@@ -2454,7 +2804,7 @@
         <v>1</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F34" s="1">
         <v>8</v>
@@ -2491,8 +2841,14 @@
         <f t="shared" si="1"/>
         <v>192</v>
       </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="U34" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="V34" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A35" s="7">
         <v>43197</v>
       </c>
@@ -2506,7 +2862,7 @@
         <v>1</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F35" s="1">
         <v>9</v>
@@ -2543,8 +2899,17 @@
         <f t="shared" si="1"/>
         <v>192</v>
       </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="U35" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="V35" s="24">
+        <v>1</v>
+      </c>
+      <c r="W35" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A36" s="7">
         <v>43197</v>
       </c>
@@ -2558,7 +2923,7 @@
         <v>1</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F36" s="1">
         <v>10</v>
@@ -2595,8 +2960,17 @@
         <f t="shared" si="1"/>
         <v>192</v>
       </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="U36" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="V36" s="24">
+        <v>1</v>
+      </c>
+      <c r="W36" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A37" s="7">
         <v>43197</v>
       </c>
@@ -2610,7 +2984,7 @@
         <v>1</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F37" s="1">
         <v>11</v>
@@ -2647,8 +3021,17 @@
         <f t="shared" si="1"/>
         <v>192</v>
       </c>
-    </row>
-    <row r="38" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U37" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="V37" s="24">
+        <v>1</v>
+      </c>
+      <c r="W37" s="24" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="8">
         <v>43197</v>
       </c>
@@ -2662,7 +3045,7 @@
         <v>1</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F38" s="9">
         <v>12</v>
@@ -2699,8 +3082,14 @@
         <f t="shared" si="1"/>
         <v>192</v>
       </c>
-    </row>
-    <row r="39" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U38" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="V38" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:24" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4">
         <v>43197</v>
       </c>
@@ -2714,7 +3103,7 @@
         <v>2</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F39" s="5">
         <v>13</v>
@@ -2751,8 +3140,14 @@
         <f t="shared" si="1"/>
         <v>133</v>
       </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="U39" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="V39" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A40" s="7">
         <v>43197</v>
       </c>
@@ -2766,7 +3161,7 @@
         <v>2</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F40" s="1">
         <v>14</v>
@@ -2803,8 +3198,20 @@
         <f t="shared" si="1"/>
         <v>133</v>
       </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="U40" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="V40" s="24">
+        <v>1</v>
+      </c>
+      <c r="W40" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="X40" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A41" s="7">
         <v>43197</v>
       </c>
@@ -2818,7 +3225,7 @@
         <v>2</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F41" s="1">
         <v>15</v>
@@ -2855,8 +3262,14 @@
         <f t="shared" si="1"/>
         <v>133</v>
       </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="U41" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="V41" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A42" s="7">
         <v>43197</v>
       </c>
@@ -2870,7 +3283,7 @@
         <v>2</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F42" s="1">
         <v>16</v>
@@ -2907,8 +3320,14 @@
         <f t="shared" si="1"/>
         <v>133</v>
       </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="U42" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="V42" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A43" s="7">
         <v>43197</v>
       </c>
@@ -2922,7 +3341,7 @@
         <v>2</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F43" s="1">
         <v>17</v>
@@ -2959,8 +3378,14 @@
         <f t="shared" si="1"/>
         <v>133</v>
       </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="U43" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="V43" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A44" s="7">
         <v>43197</v>
       </c>
@@ -2974,7 +3399,7 @@
         <v>2</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F44" s="1">
         <v>18</v>
@@ -3011,8 +3436,17 @@
         <f t="shared" si="1"/>
         <v>133</v>
       </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="U44" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="V44" s="24">
+        <v>0</v>
+      </c>
+      <c r="X44" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A45" s="7">
         <v>43197</v>
       </c>
@@ -3026,7 +3460,7 @@
         <v>2</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F45" s="1">
         <v>19</v>
@@ -3063,8 +3497,14 @@
         <f t="shared" si="1"/>
         <v>133</v>
       </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="U45" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="V45" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A46" s="7">
         <v>43197</v>
       </c>
@@ -3078,7 +3518,7 @@
         <v>2</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F46" s="1">
         <v>20</v>
@@ -3115,8 +3555,17 @@
         <f t="shared" si="1"/>
         <v>133</v>
       </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="U46" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="V46" s="24">
+        <v>1</v>
+      </c>
+      <c r="W46" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A47" s="7">
         <v>43197</v>
       </c>
@@ -3130,7 +3579,7 @@
         <v>2</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F47" s="1">
         <v>21</v>
@@ -3167,8 +3616,14 @@
         <f t="shared" si="1"/>
         <v>133</v>
       </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="U47" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="V47" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A48" s="7">
         <v>43197</v>
       </c>
@@ -3182,7 +3637,7 @@
         <v>2</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F48" s="1">
         <v>22</v>
@@ -3219,8 +3674,14 @@
         <f t="shared" si="1"/>
         <v>133</v>
       </c>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="U48" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="V48" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A49" s="7">
         <v>43197</v>
       </c>
@@ -3234,7 +3695,7 @@
         <v>2</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F49" s="1">
         <v>23</v>
@@ -3271,8 +3732,14 @@
         <f t="shared" si="1"/>
         <v>133</v>
       </c>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="U49" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="V49" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A50" s="7">
         <v>43197</v>
       </c>
@@ -3286,7 +3753,7 @@
         <v>2</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F50" s="1">
         <v>24</v>
@@ -3323,8 +3790,14 @@
         <f t="shared" si="1"/>
         <v>133</v>
       </c>
-    </row>
-    <row r="51" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U50" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="V50" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="8">
         <v>43197</v>
       </c>
@@ -3338,7 +3811,7 @@
         <v>2</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F51" s="9">
         <v>25</v>
@@ -3375,8 +3848,14 @@
         <f t="shared" si="1"/>
         <v>133</v>
       </c>
-    </row>
-    <row r="52" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U51" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="V51" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="4">
         <v>43198</v>
       </c>
@@ -3390,7 +3869,7 @@
         <v>1</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F52" s="5">
         <v>1</v>
@@ -3408,7 +3887,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A53" s="7">
         <v>43198</v>
       </c>
@@ -3422,7 +3901,7 @@
         <v>1</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F53" s="1">
         <v>2</v>
@@ -3440,7 +3919,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A54" s="7">
         <v>43198</v>
       </c>
@@ -3454,7 +3933,7 @@
         <v>1</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F54" s="1">
         <v>3</v>
@@ -3472,7 +3951,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A55" s="7">
         <v>43198</v>
       </c>
@@ -3486,7 +3965,7 @@
         <v>1</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F55" s="1">
         <v>4</v>
@@ -3504,7 +3983,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A56" s="7">
         <v>43198</v>
       </c>
@@ -3518,7 +3997,7 @@
         <v>1</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F56" s="1">
         <v>5</v>
@@ -3536,7 +4015,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A57" s="7">
         <v>43198</v>
       </c>
@@ -3550,7 +4029,7 @@
         <v>1</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F57" s="1">
         <v>6</v>
@@ -3568,7 +4047,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A58" s="7">
         <v>43198</v>
       </c>
@@ -3582,7 +4061,7 @@
         <v>1</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F58" s="1">
         <v>7</v>
@@ -3600,7 +4079,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A59" s="7">
         <v>43198</v>
       </c>
@@ -3614,7 +4093,7 @@
         <v>1</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F59" s="1">
         <v>8</v>
@@ -3632,7 +4111,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A60" s="7">
         <v>43198</v>
       </c>
@@ -3646,7 +4125,7 @@
         <v>1</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F60" s="1">
         <v>9</v>
@@ -3664,7 +4143,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A61" s="7">
         <v>43198</v>
       </c>
@@ -3678,7 +4157,7 @@
         <v>1</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F61" s="1">
         <v>10</v>
@@ -3696,7 +4175,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A62" s="7">
         <v>43198</v>
       </c>
@@ -3710,7 +4189,7 @@
         <v>1</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F62" s="1">
         <v>11</v>
@@ -3728,7 +4207,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="63" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="8">
         <v>43198</v>
       </c>
@@ -3742,7 +4221,7 @@
         <v>1</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F63" s="9">
         <v>12</v>
@@ -3760,7 +4239,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="64" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:22" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="4">
         <v>43198</v>
       </c>
@@ -3774,7 +4253,7 @@
         <v>2</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F64" s="5">
         <v>13</v>
@@ -3806,7 +4285,7 @@
         <v>2</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F65" s="1">
         <v>14</v>
@@ -3838,7 +4317,7 @@
         <v>2</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F66" s="1">
         <v>15</v>
@@ -3870,7 +4349,7 @@
         <v>2</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F67" s="1">
         <v>16</v>
@@ -3902,7 +4381,7 @@
         <v>2</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F68" s="1">
         <v>17</v>
@@ -3934,7 +4413,7 @@
         <v>2</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F69" s="1">
         <v>18</v>
@@ -3966,7 +4445,7 @@
         <v>2</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F70" s="1">
         <v>19</v>
@@ -3998,7 +4477,7 @@
         <v>2</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F71" s="1">
         <v>20</v>
@@ -4030,7 +4509,7 @@
         <v>2</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F72" s="1">
         <v>21</v>
@@ -4062,7 +4541,7 @@
         <v>2</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F73" s="1">
         <v>22</v>
@@ -4094,7 +4573,7 @@
         <v>2</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F74" s="1">
         <v>23</v>
@@ -4126,7 +4605,7 @@
         <v>2</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F75" s="1">
         <v>24</v>
@@ -4158,7 +4637,7 @@
         <v>2</v>
       </c>
       <c r="E76" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F76" s="9">
         <v>25</v>
@@ -4190,7 +4669,7 @@
         <v>1</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F77" s="5">
         <v>1</v>
@@ -4222,7 +4701,7 @@
         <v>1</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F78" s="1">
         <v>2</v>
@@ -4254,7 +4733,7 @@
         <v>1</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F79" s="1">
         <v>3</v>
@@ -4286,7 +4765,7 @@
         <v>1</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F80" s="1">
         <v>4</v>
@@ -4318,7 +4797,7 @@
         <v>1</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F81" s="1">
         <v>5</v>
@@ -4350,7 +4829,7 @@
         <v>1</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F82" s="1">
         <v>6</v>
@@ -4382,7 +4861,7 @@
         <v>1</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F83" s="1">
         <v>7</v>
@@ -4414,7 +4893,7 @@
         <v>1</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F84" s="1">
         <v>8</v>
@@ -4446,7 +4925,7 @@
         <v>1</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F85" s="1">
         <v>9</v>
@@ -4478,7 +4957,7 @@
         <v>1</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F86" s="1">
         <v>10</v>
@@ -4510,7 +4989,7 @@
         <v>1</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F87" s="1">
         <v>11</v>
@@ -4542,7 +5021,7 @@
         <v>1</v>
       </c>
       <c r="E88" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F88" s="9">
         <v>12</v>
@@ -4574,7 +5053,7 @@
         <v>2</v>
       </c>
       <c r="E89" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F89" s="5">
         <v>13</v>
@@ -4606,7 +5085,7 @@
         <v>2</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F90" s="1">
         <v>14</v>
@@ -4638,7 +5117,7 @@
         <v>2</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F91" s="1">
         <v>15</v>
@@ -4670,7 +5149,7 @@
         <v>2</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F92" s="1">
         <v>16</v>
@@ -4702,7 +5181,7 @@
         <v>2</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F93" s="1">
         <v>17</v>
@@ -4734,7 +5213,7 @@
         <v>2</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F94" s="1">
         <v>18</v>
@@ -4766,7 +5245,7 @@
         <v>2</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F95" s="1">
         <v>19</v>
@@ -4798,7 +5277,7 @@
         <v>2</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F96" s="1">
         <v>20</v>
@@ -4829,7 +5308,7 @@
         <v>2</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F97" s="1">
         <v>21</v>
@@ -4860,7 +5339,7 @@
         <v>2</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F98" s="1">
         <v>22</v>
@@ -4891,7 +5370,7 @@
         <v>2</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F99" s="1">
         <v>23</v>
@@ -4922,7 +5401,7 @@
         <v>2</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F100" s="1">
         <v>24</v>
@@ -4953,7 +5432,7 @@
         <v>2</v>
       </c>
       <c r="E101" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F101" s="9">
         <v>25</v>

</xml_diff>

<commit_message>
added today’s ch mass and Tbs
</commit_message>
<xml_diff>
--- a/data/curve_data/ldeli_tinc_integrate.xlsx
+++ b/data/curve_data/ldeli_tinc_integrate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fontikar/Dropbox/Ldeli_inc_metabTelo/data/curve_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAE22156-4FA1-684F-A3B6-7508E6A9D331}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B66E479B-E12B-2245-8AD6-90D14DC10878}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1980" yWindow="1800" windowWidth="36360" windowHeight="16940" xr2:uid="{84C113A7-A3A6-0745-8C21-C9F341A27D93}"/>
   </bookViews>
@@ -328,7 +328,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -409,12 +409,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -422,27 +440,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -461,13 +470,33 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Accent3" xfId="1" builtinId="38"/>
@@ -786,157 +815,157 @@
   <dimension ref="A1:Y101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W27" sqref="W27:X51"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O90" sqref="O90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="3"/>
-    <col min="2" max="2" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="10.83203125" style="3"/>
-    <col min="8" max="8" width="12.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="3"/>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="10.83203125" style="1"/>
+    <col min="8" max="8" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="17" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:25" s="8" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="17" t="s">
+      <c r="C1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="J1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="K1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="18" t="s">
+      <c r="L1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="18" t="s">
+      <c r="M1" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="N1" s="19" t="s">
+      <c r="N1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="19" t="s">
+      <c r="O1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="20" t="s">
+      <c r="P1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="23" t="s">
+      <c r="Q1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="21" t="s">
+      <c r="R1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="21" t="s">
+      <c r="S1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="21" t="s">
+      <c r="T1" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="21" t="s">
+      <c r="U1" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="V1" s="17" t="s">
+      <c r="V1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="W1" s="22" t="s">
+      <c r="W1" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="X1" s="17" t="s">
+      <c r="X1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="Y1" s="17" t="s">
+      <c r="Y1" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:25" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4">
+    <row r="2" spans="1:25" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="14">
         <v>43197</v>
       </c>
-      <c r="B2" s="5">
-        <v>1</v>
-      </c>
-      <c r="C2" s="5">
-        <v>1</v>
-      </c>
-      <c r="D2" s="5">
-        <v>1</v>
-      </c>
-      <c r="E2" s="5" t="s">
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="5">
-        <v>1</v>
-      </c>
-      <c r="G2" s="5">
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3">
         <v>29</v>
       </c>
-      <c r="H2" s="6">
-        <v>1</v>
-      </c>
-      <c r="I2" s="6">
+      <c r="H2" s="4">
+        <v>1</v>
+      </c>
+      <c r="I2" s="4">
         <v>30</v>
       </c>
-      <c r="J2" s="6">
+      <c r="J2" s="4">
         <v>25.1</v>
       </c>
-      <c r="K2" s="6">
+      <c r="K2" s="4">
         <v>17.271999999999998</v>
       </c>
-      <c r="L2" s="6">
+      <c r="L2" s="4">
         <v>17.451000000000001</v>
       </c>
-      <c r="M2" s="6">
+      <c r="M2" s="4">
         <f>L2-K2</f>
         <v>0.17900000000000205</v>
       </c>
-      <c r="N2" s="14">
+      <c r="N2" s="15">
         <v>0.33680555555555558</v>
       </c>
-      <c r="O2" s="14">
+      <c r="O2" s="15">
         <v>0.4284722222222222</v>
       </c>
-      <c r="P2" s="14" t="str">
+      <c r="P2" s="15" t="str">
         <f>TEXT(O2-N2, "[mm]")</f>
         <v>132</v>
       </c>
-      <c r="Q2" s="3"/>
-      <c r="U2" s="11" t="s">
+      <c r="Q2" s="1"/>
+      <c r="U2" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="V2" s="11">
+      <c r="V2" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A3" s="7">
+      <c r="A3" s="16">
         <v>43197</v>
       </c>
       <c r="B3" s="1">
@@ -976,28 +1005,28 @@
         <f t="shared" ref="M3:M26" si="0">L3-K3</f>
         <v>0.21900000000000119</v>
       </c>
-      <c r="N3" s="13">
+      <c r="N3" s="17">
         <v>0.33749999999999997</v>
       </c>
-      <c r="O3" s="13">
+      <c r="O3" s="17">
         <v>0.4291666666666667</v>
       </c>
-      <c r="P3" s="13" t="str">
+      <c r="P3" s="17" t="str">
         <f t="shared" ref="P3:P66" si="1">TEXT(O3-N3, "[mm]")</f>
         <v>132</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="U3" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="V3" s="3">
+      <c r="V3" s="1">
         <v>0</v>
       </c>
-      <c r="W3" s="3" t="s">
+      <c r="W3" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A4" s="7">
+      <c r="A4" s="16">
         <v>43197</v>
       </c>
       <c r="B4" s="1">
@@ -1037,28 +1066,28 @@
         <f t="shared" si="0"/>
         <v>0.18900000000000006</v>
       </c>
-      <c r="N4" s="13">
+      <c r="N4" s="17">
         <v>0.33819444444444402</v>
       </c>
-      <c r="O4" s="13">
+      <c r="O4" s="17">
         <v>0.42986111111111103</v>
       </c>
-      <c r="P4" s="13" t="str">
+      <c r="P4" s="17" t="str">
         <f t="shared" si="1"/>
         <v>132</v>
       </c>
-      <c r="U4" s="3" t="s">
+      <c r="U4" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="V4" s="3">
-        <v>1</v>
-      </c>
-      <c r="X4" s="3" t="s">
+      <c r="V4" s="1">
+        <v>1</v>
+      </c>
+      <c r="X4" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A5" s="7">
+      <c r="A5" s="16">
         <v>43197</v>
       </c>
       <c r="B5" s="1">
@@ -1098,25 +1127,25 @@
         <f t="shared" si="0"/>
         <v>0.22700000000000031</v>
       </c>
-      <c r="N5" s="13">
+      <c r="N5" s="17">
         <v>0.33888888888888902</v>
       </c>
-      <c r="O5" s="13">
+      <c r="O5" s="17">
         <v>0.43055555555555602</v>
       </c>
-      <c r="P5" s="13" t="str">
+      <c r="P5" s="17" t="str">
         <f t="shared" si="1"/>
         <v>132</v>
       </c>
-      <c r="U5" s="24" t="s">
+      <c r="U5" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="V5" s="24">
+      <c r="V5" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A6" s="7">
+      <c r="A6" s="16">
         <v>43197</v>
       </c>
       <c r="B6" s="1">
@@ -1156,25 +1185,25 @@
         <f t="shared" si="0"/>
         <v>0.21199999999999974</v>
       </c>
-      <c r="N6" s="13">
+      <c r="N6" s="17">
         <v>0.33958333333333302</v>
       </c>
-      <c r="O6" s="13">
+      <c r="O6" s="17">
         <v>0.43125000000000002</v>
       </c>
-      <c r="P6" s="13" t="str">
+      <c r="P6" s="17" t="str">
         <f t="shared" si="1"/>
         <v>132</v>
       </c>
-      <c r="U6" s="24" t="s">
+      <c r="U6" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="V6" s="24">
+      <c r="V6" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A7" s="7">
+      <c r="A7" s="16">
         <v>43197</v>
       </c>
       <c r="B7" s="1">
@@ -1214,31 +1243,31 @@
         <f t="shared" si="0"/>
         <v>0.20300000000000296</v>
       </c>
-      <c r="N7" s="13">
+      <c r="N7" s="17">
         <v>0.34027777777777801</v>
       </c>
-      <c r="O7" s="13">
+      <c r="O7" s="17">
         <v>0.43194444444444502</v>
       </c>
-      <c r="P7" s="13" t="str">
+      <c r="P7" s="17" t="str">
         <f t="shared" si="1"/>
         <v>132</v>
       </c>
-      <c r="U7" s="24" t="s">
+      <c r="U7" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="V7" s="24">
+      <c r="V7" s="2">
         <v>0</v>
       </c>
-      <c r="W7" s="3" t="s">
+      <c r="W7" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="X7" s="3" t="s">
+      <c r="X7" s="1" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A8" s="7">
+      <c r="A8" s="16">
         <v>43197</v>
       </c>
       <c r="B8" s="1">
@@ -1278,31 +1307,31 @@
         <f t="shared" si="0"/>
         <v>0.22800000000000153</v>
       </c>
-      <c r="N8" s="13">
+      <c r="N8" s="17">
         <v>0.34097222222222201</v>
       </c>
-      <c r="O8" s="13">
+      <c r="O8" s="17">
         <v>0.43263888888888902</v>
       </c>
-      <c r="P8" s="13" t="str">
+      <c r="P8" s="17" t="str">
         <f t="shared" si="1"/>
         <v>132</v>
       </c>
-      <c r="U8" s="24" t="s">
+      <c r="U8" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="V8" s="24">
-        <v>1</v>
-      </c>
-      <c r="W8" s="3" t="s">
+      <c r="V8" s="2">
+        <v>1</v>
+      </c>
+      <c r="W8" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="X8" s="3" t="s">
+      <c r="X8" s="1" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A9" s="7">
+      <c r="A9" s="16">
         <v>43197</v>
       </c>
       <c r="B9" s="1">
@@ -1342,25 +1371,25 @@
         <f t="shared" si="0"/>
         <v>0.21999999999999886</v>
       </c>
-      <c r="N9" s="13">
+      <c r="N9" s="17">
         <v>0.34166666666666601</v>
       </c>
-      <c r="O9" s="13">
+      <c r="O9" s="17">
         <v>0.43333333333333401</v>
       </c>
-      <c r="P9" s="13" t="str">
+      <c r="P9" s="17" t="str">
         <f t="shared" si="1"/>
         <v>132</v>
       </c>
-      <c r="U9" s="24" t="s">
+      <c r="U9" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="V9" s="24">
+      <c r="V9" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A10" s="7">
+      <c r="A10" s="16">
         <v>43197</v>
       </c>
       <c r="B10" s="1">
@@ -1400,28 +1429,28 @@
         <f t="shared" si="0"/>
         <v>0.22500000000000142</v>
       </c>
-      <c r="N10" s="13">
+      <c r="N10" s="17">
         <v>0.34236111111111101</v>
       </c>
-      <c r="O10" s="13">
+      <c r="O10" s="17">
         <v>0.43402777777777801</v>
       </c>
-      <c r="P10" s="13" t="str">
+      <c r="P10" s="17" t="str">
         <f t="shared" si="1"/>
         <v>132</v>
       </c>
-      <c r="U10" s="24" t="s">
+      <c r="U10" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="V10" s="24">
-        <v>1</v>
-      </c>
-      <c r="W10" s="3" t="s">
+      <c r="V10" s="2">
+        <v>1</v>
+      </c>
+      <c r="W10" s="1" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A11" s="7">
+      <c r="A11" s="16">
         <v>43197</v>
       </c>
       <c r="B11" s="1">
@@ -1461,28 +1490,28 @@
         <f t="shared" si="0"/>
         <v>0.23199999999999932</v>
       </c>
-      <c r="N11" s="13">
+      <c r="N11" s="17">
         <v>0.343055555555555</v>
       </c>
-      <c r="O11" s="13">
+      <c r="O11" s="17">
         <v>0.43472222222222301</v>
       </c>
-      <c r="P11" s="13" t="str">
+      <c r="P11" s="17" t="str">
         <f t="shared" si="1"/>
         <v>132</v>
       </c>
-      <c r="U11" s="24" t="s">
+      <c r="U11" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="V11" s="24">
-        <v>1</v>
-      </c>
-      <c r="W11" s="3" t="s">
+      <c r="V11" s="2">
+        <v>1</v>
+      </c>
+      <c r="W11" s="1" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A12" s="7">
+      <c r="A12" s="16">
         <v>43197</v>
       </c>
       <c r="B12" s="1">
@@ -1522,144 +1551,144 @@
         <f t="shared" si="0"/>
         <v>0.2289999999999992</v>
       </c>
-      <c r="N12" s="13">
+      <c r="N12" s="17">
         <v>0.343749999999999</v>
       </c>
-      <c r="O12" s="13">
+      <c r="O12" s="17">
         <v>0.43541666666666701</v>
       </c>
-      <c r="P12" s="13" t="str">
+      <c r="P12" s="17" t="str">
         <f t="shared" si="1"/>
         <v>132</v>
       </c>
-      <c r="U12" s="24" t="s">
+      <c r="U12" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="V12" s="24">
-        <v>1</v>
-      </c>
-      <c r="W12" s="24" t="s">
+      <c r="V12" s="2">
+        <v>1</v>
+      </c>
+      <c r="W12" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:25" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="8">
+    <row r="13" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="18">
         <v>43197</v>
       </c>
-      <c r="B13" s="9">
-        <v>1</v>
-      </c>
-      <c r="C13" s="9">
-        <v>1</v>
-      </c>
-      <c r="D13" s="9">
-        <v>1</v>
-      </c>
-      <c r="E13" s="9" t="s">
+      <c r="B13" s="5">
+        <v>1</v>
+      </c>
+      <c r="C13" s="5">
+        <v>1</v>
+      </c>
+      <c r="D13" s="5">
+        <v>1</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="5">
         <v>12</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="5">
         <v>23</v>
       </c>
-      <c r="H13" s="10">
-        <v>1</v>
-      </c>
-      <c r="I13" s="10">
+      <c r="H13" s="6">
+        <v>1</v>
+      </c>
+      <c r="I13" s="6">
         <v>30</v>
       </c>
-      <c r="J13" s="10">
+      <c r="J13" s="6">
         <v>25.6</v>
       </c>
-      <c r="K13" s="10">
+      <c r="K13" s="6">
         <v>17.071999999999999</v>
       </c>
-      <c r="L13" s="10">
+      <c r="L13" s="6">
         <v>17.280999999999999</v>
       </c>
-      <c r="M13" s="10">
+      <c r="M13" s="6">
         <f t="shared" si="0"/>
         <v>0.20899999999999963</v>
       </c>
-      <c r="N13" s="15">
+      <c r="N13" s="19">
         <v>0.344444444444444</v>
       </c>
-      <c r="O13" s="15">
+      <c r="O13" s="19">
         <v>0.436111111111112</v>
       </c>
-      <c r="P13" s="15" t="str">
+      <c r="P13" s="19" t="str">
         <f t="shared" si="1"/>
         <v>132</v>
       </c>
-      <c r="U13" s="12" t="s">
+      <c r="U13" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="V13" s="12">
+      <c r="V13" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:25" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="4">
+    <row r="14" spans="1:25" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="14">
         <v>43197</v>
       </c>
-      <c r="B14" s="5">
-        <v>1</v>
-      </c>
-      <c r="C14" s="5">
-        <v>1</v>
-      </c>
-      <c r="D14" s="5">
+      <c r="B14" s="3">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1</v>
+      </c>
+      <c r="D14" s="3">
         <v>2</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="3">
         <v>13</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="3">
         <v>23</v>
       </c>
-      <c r="H14" s="6">
-        <v>1</v>
-      </c>
-      <c r="I14" s="6">
+      <c r="H14" s="4">
+        <v>1</v>
+      </c>
+      <c r="I14" s="4">
         <v>24</v>
       </c>
-      <c r="J14" s="6">
+      <c r="J14" s="4">
         <v>24.2</v>
       </c>
-      <c r="K14" s="6">
+      <c r="K14" s="4">
         <v>17.206</v>
       </c>
-      <c r="L14" s="6">
+      <c r="L14" s="4">
         <v>17.358000000000001</v>
       </c>
-      <c r="M14" s="6">
+      <c r="M14" s="4">
         <f t="shared" si="0"/>
         <v>0.15200000000000102</v>
       </c>
-      <c r="N14" s="14">
+      <c r="N14" s="15">
         <v>0.35694444444444445</v>
       </c>
-      <c r="O14" s="14">
+      <c r="O14" s="15">
         <v>0.4909722222222222</v>
       </c>
-      <c r="P14" s="14" t="str">
+      <c r="P14" s="15" t="str">
         <f t="shared" si="1"/>
         <v>193</v>
       </c>
-      <c r="U14" s="11" t="s">
+      <c r="U14" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="V14" s="11">
+      <c r="V14" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A15" s="7">
+      <c r="A15" s="16">
         <v>43197</v>
       </c>
       <c r="B15" s="1">
@@ -1699,31 +1728,31 @@
         <f t="shared" si="0"/>
         <v>0.23400000000000176</v>
       </c>
-      <c r="N15" s="13">
+      <c r="N15" s="17">
         <v>0.3576388888888889</v>
       </c>
-      <c r="O15" s="13">
+      <c r="O15" s="17">
         <v>0.4916666666666667</v>
       </c>
-      <c r="P15" s="13" t="str">
+      <c r="P15" s="17" t="str">
         <f t="shared" si="1"/>
         <v>193</v>
       </c>
-      <c r="U15" s="24" t="s">
+      <c r="U15" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="V15" s="24">
-        <v>1</v>
-      </c>
-      <c r="W15" s="3" t="s">
+      <c r="V15" s="2">
+        <v>1</v>
+      </c>
+      <c r="W15" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="X15" s="3" t="s">
+      <c r="X15" s="1" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A16" s="7">
+      <c r="A16" s="16">
         <v>43197</v>
       </c>
       <c r="B16" s="1">
@@ -1763,25 +1792,25 @@
         <f t="shared" si="0"/>
         <v>0.20599999999999952</v>
       </c>
-      <c r="N16" s="13">
+      <c r="N16" s="17">
         <v>0.358333333333333</v>
       </c>
-      <c r="O16" s="13">
+      <c r="O16" s="17">
         <v>0.49236111111111103</v>
       </c>
-      <c r="P16" s="13" t="str">
+      <c r="P16" s="17" t="str">
         <f t="shared" si="1"/>
         <v>193</v>
       </c>
-      <c r="U16" s="24" t="s">
+      <c r="U16" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="V16" s="24">
+      <c r="V16" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A17" s="7">
+      <c r="A17" s="16">
         <v>43197</v>
       </c>
       <c r="B17" s="1">
@@ -1821,25 +1850,25 @@
         <f t="shared" si="0"/>
         <v>0.23600000000000065</v>
       </c>
-      <c r="N17" s="13">
+      <c r="N17" s="17">
         <v>0.359027777777778</v>
       </c>
-      <c r="O17" s="13">
+      <c r="O17" s="17">
         <v>0.49305555555555602</v>
       </c>
-      <c r="P17" s="13" t="str">
+      <c r="P17" s="17" t="str">
         <f t="shared" si="1"/>
         <v>193</v>
       </c>
-      <c r="U17" s="24" t="s">
+      <c r="U17" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="V17" s="24">
+      <c r="V17" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A18" s="7">
+      <c r="A18" s="16">
         <v>43197</v>
       </c>
       <c r="B18" s="1">
@@ -1879,25 +1908,25 @@
         <f t="shared" si="0"/>
         <v>0.22500000000000142</v>
       </c>
-      <c r="N18" s="13">
+      <c r="N18" s="17">
         <v>0.359722222222222</v>
       </c>
-      <c r="O18" s="13">
+      <c r="O18" s="17">
         <v>0.49375000000000002</v>
       </c>
-      <c r="P18" s="13" t="str">
+      <c r="P18" s="17" t="str">
         <f t="shared" si="1"/>
         <v>193</v>
       </c>
-      <c r="U18" s="24" t="s">
+      <c r="U18" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="V18" s="24">
+      <c r="V18" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A19" s="7">
+      <c r="A19" s="16">
         <v>43197</v>
       </c>
       <c r="B19" s="1">
@@ -1937,28 +1966,28 @@
         <f t="shared" si="0"/>
         <v>0.20800000000000196</v>
       </c>
-      <c r="N19" s="13">
+      <c r="N19" s="17">
         <v>0.360416666666667</v>
       </c>
-      <c r="O19" s="13">
+      <c r="O19" s="17">
         <v>0.49444444444444502</v>
       </c>
-      <c r="P19" s="13" t="str">
+      <c r="P19" s="17" t="str">
         <f t="shared" si="1"/>
         <v>193</v>
       </c>
-      <c r="U19" s="24" t="s">
+      <c r="U19" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="V19" s="24">
+      <c r="V19" s="2">
         <v>0</v>
       </c>
-      <c r="X19" s="3" t="s">
+      <c r="X19" s="1" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A20" s="7">
+      <c r="A20" s="16">
         <v>43197</v>
       </c>
       <c r="B20" s="1">
@@ -1998,25 +2027,25 @@
         <f t="shared" si="0"/>
         <v>0.18200000000000216</v>
       </c>
-      <c r="N20" s="13">
+      <c r="N20" s="17">
         <v>0.36111111111111099</v>
       </c>
-      <c r="O20" s="13">
+      <c r="O20" s="17">
         <v>0.49513888888888902</v>
       </c>
-      <c r="P20" s="13" t="str">
+      <c r="P20" s="17" t="str">
         <f t="shared" si="1"/>
         <v>193</v>
       </c>
-      <c r="U20" s="24" t="s">
+      <c r="U20" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="V20" s="24">
+      <c r="V20" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A21" s="7">
+      <c r="A21" s="16">
         <v>43197</v>
       </c>
       <c r="B21" s="1">
@@ -2056,28 +2085,28 @@
         <f t="shared" si="0"/>
         <v>0.21999999999999886</v>
       </c>
-      <c r="N21" s="13">
+      <c r="N21" s="17">
         <v>0.36180555555555599</v>
       </c>
-      <c r="O21" s="13">
+      <c r="O21" s="17">
         <v>0.49583333333333401</v>
       </c>
-      <c r="P21" s="13" t="str">
+      <c r="P21" s="17" t="str">
         <f t="shared" si="1"/>
         <v>193</v>
       </c>
-      <c r="U21" s="24" t="s">
+      <c r="U21" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="V21" s="24">
-        <v>1</v>
-      </c>
-      <c r="W21" s="3" t="s">
+      <c r="V21" s="2">
+        <v>1</v>
+      </c>
+      <c r="W21" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A22" s="7">
+      <c r="A22" s="16">
         <v>43197</v>
       </c>
       <c r="B22" s="1">
@@ -2117,25 +2146,25 @@
         <f t="shared" si="0"/>
         <v>0.22200000000000131</v>
       </c>
-      <c r="N22" s="13">
+      <c r="N22" s="17">
         <v>0.36249999999999999</v>
       </c>
-      <c r="O22" s="13">
+      <c r="O22" s="17">
         <v>0.49652777777777801</v>
       </c>
-      <c r="P22" s="13" t="str">
+      <c r="P22" s="17" t="str">
         <f t="shared" si="1"/>
         <v>193</v>
       </c>
-      <c r="U22" s="24" t="s">
+      <c r="U22" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="V22" s="24">
+      <c r="V22" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A23" s="7">
+      <c r="A23" s="16">
         <v>43197</v>
       </c>
       <c r="B23" s="1">
@@ -2175,25 +2204,25 @@
         <f t="shared" si="0"/>
         <v>0.22700000000000031</v>
       </c>
-      <c r="N23" s="13">
+      <c r="N23" s="17">
         <v>0.36319444444444399</v>
       </c>
-      <c r="O23" s="13">
+      <c r="O23" s="17">
         <v>0.49722222222222301</v>
       </c>
-      <c r="P23" s="13" t="str">
+      <c r="P23" s="17" t="str">
         <f t="shared" si="1"/>
         <v>193</v>
       </c>
-      <c r="U23" s="24" t="s">
+      <c r="U23" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="V23" s="24">
+      <c r="V23" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A24" s="7">
+      <c r="A24" s="16">
         <v>43197</v>
       </c>
       <c r="B24" s="1">
@@ -2233,25 +2262,25 @@
         <f t="shared" si="0"/>
         <v>0.22299999999999898</v>
       </c>
-      <c r="N24" s="13">
+      <c r="N24" s="17">
         <v>0.36388888888888898</v>
       </c>
-      <c r="O24" s="13">
+      <c r="O24" s="17">
         <v>0.49791666666666701</v>
       </c>
-      <c r="P24" s="13" t="str">
+      <c r="P24" s="17" t="str">
         <f t="shared" si="1"/>
         <v>193</v>
       </c>
-      <c r="U24" s="24" t="s">
+      <c r="U24" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="V24" s="24">
+      <c r="V24" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A25" s="7">
+      <c r="A25" s="16">
         <v>43197</v>
       </c>
       <c r="B25" s="1">
@@ -2291,141 +2320,141 @@
         <f t="shared" si="0"/>
         <v>0.24099999999999966</v>
       </c>
-      <c r="N25" s="13">
+      <c r="N25" s="17">
         <v>0.36458333333333298</v>
       </c>
-      <c r="O25" s="13">
+      <c r="O25" s="17">
         <v>0.498611111111112</v>
       </c>
-      <c r="P25" s="13" t="str">
+      <c r="P25" s="17" t="str">
         <f t="shared" si="1"/>
         <v>193</v>
       </c>
-      <c r="U25" s="24" t="s">
+      <c r="U25" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="V25" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:24" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="8">
+      <c r="V25" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="18">
         <v>43197</v>
       </c>
-      <c r="B26" s="9">
-        <v>1</v>
-      </c>
-      <c r="C26" s="9">
-        <v>1</v>
-      </c>
-      <c r="D26" s="9">
+      <c r="B26" s="5">
+        <v>1</v>
+      </c>
+      <c r="C26" s="5">
+        <v>1</v>
+      </c>
+      <c r="D26" s="5">
         <v>2</v>
       </c>
-      <c r="E26" s="9" t="s">
+      <c r="E26" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F26" s="9">
+      <c r="F26" s="5">
         <v>25</v>
       </c>
-      <c r="G26" s="9">
+      <c r="G26" s="5">
         <v>29</v>
       </c>
-      <c r="H26" s="10">
-        <v>1</v>
-      </c>
-      <c r="I26" s="10">
+      <c r="H26" s="6">
+        <v>1</v>
+      </c>
+      <c r="I26" s="6">
         <v>24</v>
       </c>
-      <c r="J26" s="10">
+      <c r="J26" s="6">
         <v>23.9</v>
       </c>
-      <c r="K26" s="10">
+      <c r="K26" s="6">
         <v>17.239000000000001</v>
       </c>
-      <c r="L26" s="10">
+      <c r="L26" s="6">
         <v>17.459</v>
       </c>
-      <c r="M26" s="10">
+      <c r="M26" s="6">
         <f t="shared" si="0"/>
         <v>0.21999999999999886</v>
       </c>
-      <c r="N26" s="15">
+      <c r="N26" s="19">
         <v>0.36527777777777798</v>
       </c>
-      <c r="O26" s="15">
+      <c r="O26" s="19">
         <v>0.499305555555556</v>
       </c>
-      <c r="P26" s="15" t="str">
+      <c r="P26" s="19" t="str">
         <f t="shared" si="1"/>
         <v>193</v>
       </c>
-      <c r="U26" s="12" t="s">
+      <c r="U26" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="V26" s="12">
+      <c r="V26" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:24" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="4">
+    <row r="27" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="14">
         <v>43197</v>
       </c>
-      <c r="B27" s="5">
-        <v>1</v>
-      </c>
-      <c r="C27" s="5">
-        <v>1</v>
-      </c>
-      <c r="D27" s="5">
-        <v>1</v>
-      </c>
-      <c r="E27" s="5" t="s">
+      <c r="B27" s="3">
+        <v>1</v>
+      </c>
+      <c r="C27" s="3">
+        <v>1</v>
+      </c>
+      <c r="D27" s="3">
+        <v>1</v>
+      </c>
+      <c r="E27" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F27" s="5">
-        <v>1</v>
-      </c>
-      <c r="G27" s="5">
+      <c r="F27" s="3">
+        <v>1</v>
+      </c>
+      <c r="G27" s="3">
         <v>29</v>
       </c>
-      <c r="H27" s="6">
-        <v>1</v>
-      </c>
-      <c r="I27" s="6">
+      <c r="H27" s="4">
+        <v>1</v>
+      </c>
+      <c r="I27" s="4">
         <v>26</v>
       </c>
-      <c r="J27" s="6">
+      <c r="J27" s="4">
         <v>25.1</v>
       </c>
-      <c r="K27" s="6">
+      <c r="K27" s="4">
         <v>17.271999999999998</v>
       </c>
-      <c r="L27" s="6">
+      <c r="L27" s="4">
         <v>17.451000000000001</v>
       </c>
-      <c r="M27" s="6">
+      <c r="M27" s="4">
         <f>L27-K27</f>
         <v>0.17900000000000205</v>
       </c>
-      <c r="N27" s="14">
+      <c r="N27" s="15">
         <v>0.47152777777777777</v>
       </c>
-      <c r="O27" s="14">
+      <c r="O27" s="15">
         <v>0.60486111111111118</v>
       </c>
-      <c r="P27" s="14" t="str">
+      <c r="P27" s="15" t="str">
         <f t="shared" si="1"/>
         <v>192</v>
       </c>
-      <c r="U27" s="11" t="s">
+      <c r="U27" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="V27" s="11">
+      <c r="V27" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A28" s="7">
+      <c r="A28" s="16">
         <v>43197</v>
       </c>
       <c r="B28" s="1">
@@ -2462,31 +2491,31 @@
         <v>17.195</v>
       </c>
       <c r="M28" s="2">
-        <f t="shared" ref="M28:M51" si="2">L28-K28</f>
+        <f t="shared" ref="M28:M76" si="2">L28-K28</f>
         <v>0.21900000000000119</v>
       </c>
-      <c r="N28" s="13">
+      <c r="N28" s="17">
         <v>0.47222222222222227</v>
       </c>
-      <c r="O28" s="13">
+      <c r="O28" s="17">
         <v>0.60555555555555551</v>
       </c>
-      <c r="P28" s="13" t="str">
+      <c r="P28" s="17" t="str">
         <f t="shared" si="1"/>
         <v>192</v>
       </c>
-      <c r="U28" s="3" t="s">
+      <c r="U28" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="V28" s="3">
+      <c r="V28" s="1">
         <v>0</v>
       </c>
-      <c r="W28" s="3" t="s">
+      <c r="W28" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A29" s="7">
+      <c r="A29" s="16">
         <v>43197</v>
       </c>
       <c r="B29" s="1">
@@ -2526,28 +2555,28 @@
         <f t="shared" si="2"/>
         <v>0.18900000000000006</v>
       </c>
-      <c r="N29" s="13">
+      <c r="N29" s="17">
         <v>0.47291666666666698</v>
       </c>
-      <c r="O29" s="13">
+      <c r="O29" s="17">
         <v>0.60624999999999996</v>
       </c>
-      <c r="P29" s="13" t="str">
+      <c r="P29" s="17" t="str">
         <f t="shared" si="1"/>
         <v>192</v>
       </c>
-      <c r="U29" s="3" t="s">
+      <c r="U29" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="V29" s="3">
-        <v>1</v>
-      </c>
-      <c r="X29" s="3" t="s">
+      <c r="V29" s="1">
+        <v>1</v>
+      </c>
+      <c r="X29" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A30" s="7">
+      <c r="A30" s="16">
         <v>43197</v>
       </c>
       <c r="B30" s="1">
@@ -2587,25 +2616,25 @@
         <f t="shared" si="2"/>
         <v>0.22700000000000031</v>
       </c>
-      <c r="N30" s="13">
+      <c r="N30" s="17">
         <v>0.47361111111111098</v>
       </c>
-      <c r="O30" s="13">
+      <c r="O30" s="17">
         <v>0.60694444444444395</v>
       </c>
-      <c r="P30" s="13" t="str">
+      <c r="P30" s="17" t="str">
         <f t="shared" si="1"/>
         <v>192</v>
       </c>
-      <c r="U30" s="24" t="s">
+      <c r="U30" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="V30" s="24">
+      <c r="V30" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A31" s="7">
+      <c r="A31" s="16">
         <v>43197</v>
       </c>
       <c r="B31" s="1">
@@ -2645,25 +2674,25 @@
         <f t="shared" si="2"/>
         <v>0.21199999999999974</v>
       </c>
-      <c r="N31" s="13">
+      <c r="N31" s="17">
         <v>0.47430555555555598</v>
       </c>
-      <c r="O31" s="13">
+      <c r="O31" s="17">
         <v>0.60763888888888895</v>
       </c>
-      <c r="P31" s="13" t="str">
+      <c r="P31" s="17" t="str">
         <f t="shared" si="1"/>
         <v>192</v>
       </c>
-      <c r="U31" s="24" t="s">
+      <c r="U31" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="V31" s="24">
+      <c r="V31" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A32" s="7">
+      <c r="A32" s="16">
         <v>43197</v>
       </c>
       <c r="B32" s="1">
@@ -2703,31 +2732,31 @@
         <f t="shared" si="2"/>
         <v>0.20300000000000296</v>
       </c>
-      <c r="N32" s="13">
+      <c r="N32" s="17">
         <v>0.47499999999999998</v>
       </c>
-      <c r="O32" s="13">
+      <c r="O32" s="17">
         <v>0.60833333333333295</v>
       </c>
-      <c r="P32" s="13" t="str">
+      <c r="P32" s="17" t="str">
         <f t="shared" si="1"/>
         <v>192</v>
       </c>
-      <c r="U32" s="24" t="s">
+      <c r="U32" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="V32" s="24">
+      <c r="V32" s="2">
         <v>0</v>
       </c>
-      <c r="W32" s="3" t="s">
+      <c r="W32" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="X32" s="3" t="s">
+      <c r="X32" s="1" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A33" s="7">
+      <c r="A33" s="16">
         <v>43197</v>
       </c>
       <c r="B33" s="1">
@@ -2767,31 +2796,31 @@
         <f t="shared" si="2"/>
         <v>0.22800000000000153</v>
       </c>
-      <c r="N33" s="13">
+      <c r="N33" s="17">
         <v>0.47569444444444497</v>
       </c>
-      <c r="O33" s="13">
+      <c r="O33" s="17">
         <v>0.60902777777777695</v>
       </c>
-      <c r="P33" s="13" t="str">
+      <c r="P33" s="17" t="str">
         <f t="shared" si="1"/>
         <v>192</v>
       </c>
-      <c r="U33" s="24" t="s">
+      <c r="U33" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="V33" s="24">
-        <v>1</v>
-      </c>
-      <c r="W33" s="3" t="s">
+      <c r="V33" s="2">
+        <v>1</v>
+      </c>
+      <c r="W33" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="X33" s="3" t="s">
+      <c r="X33" s="1" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A34" s="7">
+      <c r="A34" s="16">
         <v>43197</v>
       </c>
       <c r="B34" s="1">
@@ -2831,25 +2860,25 @@
         <f t="shared" si="2"/>
         <v>0.21999999999999886</v>
       </c>
-      <c r="N34" s="13">
+      <c r="N34" s="17">
         <v>0.47638888888888897</v>
       </c>
-      <c r="O34" s="13">
+      <c r="O34" s="17">
         <v>0.60972222222222106</v>
       </c>
-      <c r="P34" s="13" t="str">
+      <c r="P34" s="17" t="str">
         <f t="shared" si="1"/>
         <v>192</v>
       </c>
-      <c r="U34" s="24" t="s">
+      <c r="U34" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="V34" s="24">
+      <c r="V34" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A35" s="7">
+      <c r="A35" s="16">
         <v>43197</v>
       </c>
       <c r="B35" s="1">
@@ -2889,28 +2918,28 @@
         <f t="shared" si="2"/>
         <v>0.22500000000000142</v>
       </c>
-      <c r="N35" s="13">
+      <c r="N35" s="17">
         <v>0.47708333333333403</v>
       </c>
-      <c r="O35" s="13">
+      <c r="O35" s="17">
         <v>0.61041666666666605</v>
       </c>
-      <c r="P35" s="13" t="str">
+      <c r="P35" s="17" t="str">
         <f t="shared" si="1"/>
         <v>192</v>
       </c>
-      <c r="U35" s="24" t="s">
+      <c r="U35" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="V35" s="24">
-        <v>1</v>
-      </c>
-      <c r="W35" s="3" t="s">
+      <c r="V35" s="2">
+        <v>1</v>
+      </c>
+      <c r="W35" s="1" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A36" s="7">
+      <c r="A36" s="16">
         <v>43197</v>
       </c>
       <c r="B36" s="1">
@@ -2950,28 +2979,28 @@
         <f t="shared" si="2"/>
         <v>0.23199999999999932</v>
       </c>
-      <c r="N36" s="13">
+      <c r="N36" s="17">
         <v>0.47777777777777802</v>
       </c>
-      <c r="O36" s="13">
+      <c r="O36" s="17">
         <v>0.61111111111111005</v>
       </c>
-      <c r="P36" s="13" t="str">
+      <c r="P36" s="17" t="str">
         <f t="shared" si="1"/>
         <v>192</v>
       </c>
-      <c r="U36" s="24" t="s">
+      <c r="U36" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="V36" s="24">
-        <v>1</v>
-      </c>
-      <c r="W36" s="3" t="s">
+      <c r="V36" s="2">
+        <v>1</v>
+      </c>
+      <c r="W36" s="1" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A37" s="7">
+      <c r="A37" s="16">
         <v>43197</v>
       </c>
       <c r="B37" s="1">
@@ -3011,144 +3040,144 @@
         <f t="shared" si="2"/>
         <v>0.2289999999999992</v>
       </c>
-      <c r="N37" s="13">
+      <c r="N37" s="17">
         <v>0.47847222222222302</v>
       </c>
-      <c r="O37" s="13">
+      <c r="O37" s="17">
         <v>0.61180555555555405</v>
       </c>
-      <c r="P37" s="13" t="str">
+      <c r="P37" s="17" t="str">
         <f t="shared" si="1"/>
         <v>192</v>
       </c>
-      <c r="U37" s="24" t="s">
+      <c r="U37" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="V37" s="24">
-        <v>1</v>
-      </c>
-      <c r="W37" s="24" t="s">
+      <c r="V37" s="2">
+        <v>1</v>
+      </c>
+      <c r="W37" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="38" spans="1:24" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="8">
+    <row r="38" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="18">
         <v>43197</v>
       </c>
-      <c r="B38" s="9">
-        <v>1</v>
-      </c>
-      <c r="C38" s="9">
-        <v>1</v>
-      </c>
-      <c r="D38" s="9">
-        <v>1</v>
-      </c>
-      <c r="E38" s="9" t="s">
+      <c r="B38" s="5">
+        <v>1</v>
+      </c>
+      <c r="C38" s="5">
+        <v>1</v>
+      </c>
+      <c r="D38" s="5">
+        <v>1</v>
+      </c>
+      <c r="E38" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F38" s="9">
+      <c r="F38" s="5">
         <v>12</v>
       </c>
-      <c r="G38" s="9">
+      <c r="G38" s="5">
         <v>23</v>
       </c>
-      <c r="H38" s="10">
-        <v>1</v>
-      </c>
-      <c r="I38" s="10">
+      <c r="H38" s="6">
+        <v>1</v>
+      </c>
+      <c r="I38" s="6">
         <v>26</v>
       </c>
-      <c r="J38" s="10">
+      <c r="J38" s="6">
         <v>25.6</v>
       </c>
-      <c r="K38" s="10">
+      <c r="K38" s="6">
         <v>17.071999999999999</v>
       </c>
-      <c r="L38" s="10">
+      <c r="L38" s="6">
         <v>17.280999999999999</v>
       </c>
-      <c r="M38" s="10">
+      <c r="M38" s="6">
         <f t="shared" si="2"/>
         <v>0.20899999999999963</v>
       </c>
-      <c r="N38" s="15">
+      <c r="N38" s="19">
         <v>0.47916666666666702</v>
       </c>
-      <c r="O38" s="15">
+      <c r="O38" s="19">
         <v>0.61249999999999905</v>
       </c>
-      <c r="P38" s="15" t="str">
+      <c r="P38" s="19" t="str">
         <f t="shared" si="1"/>
         <v>192</v>
       </c>
-      <c r="U38" s="12" t="s">
+      <c r="U38" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="V38" s="12">
+      <c r="V38" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:24" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="4">
+    <row r="39" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="14">
         <v>43197</v>
       </c>
-      <c r="B39" s="5">
-        <v>1</v>
-      </c>
-      <c r="C39" s="5">
-        <v>1</v>
-      </c>
-      <c r="D39" s="5">
+      <c r="B39" s="3">
+        <v>1</v>
+      </c>
+      <c r="C39" s="3">
+        <v>1</v>
+      </c>
+      <c r="D39" s="3">
         <v>2</v>
       </c>
-      <c r="E39" s="5" t="s">
+      <c r="E39" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F39" s="5">
+      <c r="F39" s="3">
         <v>13</v>
       </c>
-      <c r="G39" s="5">
+      <c r="G39" s="3">
         <v>23</v>
       </c>
-      <c r="H39" s="6">
-        <v>1</v>
-      </c>
-      <c r="I39" s="6">
+      <c r="H39" s="4">
+        <v>1</v>
+      </c>
+      <c r="I39" s="4">
         <v>34</v>
       </c>
-      <c r="J39" s="6">
+      <c r="J39" s="4">
         <v>24.2</v>
       </c>
-      <c r="K39" s="6">
+      <c r="K39" s="4">
         <v>17.206</v>
       </c>
-      <c r="L39" s="6">
+      <c r="L39" s="4">
         <v>17.358000000000001</v>
       </c>
-      <c r="M39" s="6">
+      <c r="M39" s="4">
         <f t="shared" si="2"/>
         <v>0.15200000000000102</v>
       </c>
-      <c r="N39" s="14">
+      <c r="N39" s="15">
         <v>0.53472222222222221</v>
       </c>
-      <c r="O39" s="14">
+      <c r="O39" s="15">
         <v>0.62708333333333333</v>
       </c>
-      <c r="P39" s="14" t="str">
+      <c r="P39" s="15" t="str">
         <f t="shared" si="1"/>
         <v>133</v>
       </c>
-      <c r="U39" s="11" t="s">
+      <c r="U39" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="V39" s="11">
+      <c r="V39" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A40" s="7">
+      <c r="A40" s="16">
         <v>43197</v>
       </c>
       <c r="B40" s="1">
@@ -3188,31 +3217,31 @@
         <f t="shared" si="2"/>
         <v>0.23400000000000176</v>
       </c>
-      <c r="N40" s="13">
+      <c r="N40" s="17">
         <v>0.53541666666666665</v>
       </c>
-      <c r="O40" s="13">
+      <c r="O40" s="17">
         <v>0.62777777777777777</v>
       </c>
-      <c r="P40" s="13" t="str">
+      <c r="P40" s="17" t="str">
         <f t="shared" si="1"/>
         <v>133</v>
       </c>
-      <c r="U40" s="24" t="s">
+      <c r="U40" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="V40" s="24">
-        <v>1</v>
-      </c>
-      <c r="W40" s="3" t="s">
+      <c r="V40" s="2">
+        <v>1</v>
+      </c>
+      <c r="W40" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="X40" s="3" t="s">
+      <c r="X40" s="1" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A41" s="7">
+      <c r="A41" s="16">
         <v>43197</v>
       </c>
       <c r="B41" s="1">
@@ -3252,25 +3281,25 @@
         <f t="shared" si="2"/>
         <v>0.20599999999999952</v>
       </c>
-      <c r="N41" s="13">
+      <c r="N41" s="17">
         <v>0.53611111111111098</v>
       </c>
-      <c r="O41" s="13">
+      <c r="O41" s="17">
         <v>0.62847222222222199</v>
       </c>
-      <c r="P41" s="13" t="str">
+      <c r="P41" s="17" t="str">
         <f t="shared" si="1"/>
         <v>133</v>
       </c>
-      <c r="U41" s="24" t="s">
+      <c r="U41" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="V41" s="24">
+      <c r="V41" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A42" s="7">
+      <c r="A42" s="16">
         <v>43197</v>
       </c>
       <c r="B42" s="1">
@@ -3310,25 +3339,25 @@
         <f t="shared" si="2"/>
         <v>0.23600000000000065</v>
       </c>
-      <c r="N42" s="13">
+      <c r="N42" s="17">
         <v>0.53680555555555598</v>
       </c>
-      <c r="O42" s="13">
+      <c r="O42" s="17">
         <v>0.62916666666666698</v>
       </c>
-      <c r="P42" s="13" t="str">
+      <c r="P42" s="17" t="str">
         <f t="shared" si="1"/>
         <v>133</v>
       </c>
-      <c r="U42" s="24" t="s">
+      <c r="U42" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="V42" s="24">
+      <c r="V42" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A43" s="7">
+      <c r="A43" s="16">
         <v>43197</v>
       </c>
       <c r="B43" s="1">
@@ -3368,25 +3397,25 @@
         <f t="shared" si="2"/>
         <v>0.22500000000000142</v>
       </c>
-      <c r="N43" s="13">
+      <c r="N43" s="17">
         <v>0.53749999999999998</v>
       </c>
-      <c r="O43" s="13">
+      <c r="O43" s="17">
         <v>0.62986111111111098</v>
       </c>
-      <c r="P43" s="13" t="str">
+      <c r="P43" s="17" t="str">
         <f t="shared" si="1"/>
         <v>133</v>
       </c>
-      <c r="U43" s="24" t="s">
+      <c r="U43" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="V43" s="24">
+      <c r="V43" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A44" s="7">
+      <c r="A44" s="16">
         <v>43197</v>
       </c>
       <c r="B44" s="1">
@@ -3426,28 +3455,28 @@
         <f t="shared" si="2"/>
         <v>0.20800000000000196</v>
       </c>
-      <c r="N44" s="13">
+      <c r="N44" s="17">
         <v>0.53819444444444398</v>
       </c>
-      <c r="O44" s="13">
+      <c r="O44" s="17">
         <v>0.63055555555555598</v>
       </c>
-      <c r="P44" s="13" t="str">
+      <c r="P44" s="17" t="str">
         <f t="shared" si="1"/>
         <v>133</v>
       </c>
-      <c r="U44" s="24" t="s">
+      <c r="U44" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="V44" s="24">
+      <c r="V44" s="2">
         <v>0</v>
       </c>
-      <c r="X44" s="3" t="s">
+      <c r="X44" s="1" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A45" s="7">
+      <c r="A45" s="16">
         <v>43197</v>
       </c>
       <c r="B45" s="1">
@@ -3487,25 +3516,25 @@
         <f t="shared" si="2"/>
         <v>0.18200000000000216</v>
       </c>
-      <c r="N45" s="13">
+      <c r="N45" s="17">
         <v>0.53888888888888897</v>
       </c>
-      <c r="O45" s="13">
+      <c r="O45" s="17">
         <v>0.63124999999999998</v>
       </c>
-      <c r="P45" s="13" t="str">
+      <c r="P45" s="17" t="str">
         <f t="shared" si="1"/>
         <v>133</v>
       </c>
-      <c r="U45" s="24" t="s">
+      <c r="U45" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="V45" s="24">
+      <c r="V45" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A46" s="7">
+      <c r="A46" s="16">
         <v>43197</v>
       </c>
       <c r="B46" s="1">
@@ -3545,28 +3574,28 @@
         <f t="shared" si="2"/>
         <v>0.21999999999999886</v>
       </c>
-      <c r="N46" s="13">
+      <c r="N46" s="17">
         <v>0.53958333333333297</v>
       </c>
-      <c r="O46" s="13">
+      <c r="O46" s="17">
         <v>0.63194444444444398</v>
       </c>
-      <c r="P46" s="13" t="str">
+      <c r="P46" s="17" t="str">
         <f t="shared" si="1"/>
         <v>133</v>
       </c>
-      <c r="U46" s="24" t="s">
+      <c r="U46" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="V46" s="24">
-        <v>1</v>
-      </c>
-      <c r="W46" s="3" t="s">
+      <c r="V46" s="2">
+        <v>1</v>
+      </c>
+      <c r="W46" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="47" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A47" s="7">
+      <c r="A47" s="16">
         <v>43197</v>
       </c>
       <c r="B47" s="1">
@@ -3606,25 +3635,25 @@
         <f t="shared" si="2"/>
         <v>0.22200000000000131</v>
       </c>
-      <c r="N47" s="13">
+      <c r="N47" s="17">
         <v>0.54027777777777797</v>
       </c>
-      <c r="O47" s="13">
+      <c r="O47" s="17">
         <v>0.63263888888888897</v>
       </c>
-      <c r="P47" s="13" t="str">
+      <c r="P47" s="17" t="str">
         <f t="shared" si="1"/>
         <v>133</v>
       </c>
-      <c r="U47" s="24" t="s">
+      <c r="U47" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="V47" s="24">
+      <c r="V47" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A48" s="7">
+      <c r="A48" s="16">
         <v>43197</v>
       </c>
       <c r="B48" s="1">
@@ -3664,25 +3693,25 @@
         <f t="shared" si="2"/>
         <v>0.22700000000000031</v>
       </c>
-      <c r="N48" s="13">
+      <c r="N48" s="17">
         <v>0.54097222222222197</v>
       </c>
-      <c r="O48" s="13">
+      <c r="O48" s="17">
         <v>0.63333333333333297</v>
       </c>
-      <c r="P48" s="13" t="str">
+      <c r="P48" s="17" t="str">
         <f t="shared" si="1"/>
         <v>133</v>
       </c>
-      <c r="U48" s="24" t="s">
+      <c r="U48" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="V48" s="24">
+      <c r="V48" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A49" s="7">
+      <c r="A49" s="16">
         <v>43197</v>
       </c>
       <c r="B49" s="1">
@@ -3722,25 +3751,25 @@
         <f t="shared" si="2"/>
         <v>0.22299999999999898</v>
       </c>
-      <c r="N49" s="13">
+      <c r="N49" s="17">
         <v>0.54166666666666696</v>
       </c>
-      <c r="O49" s="13">
+      <c r="O49" s="17">
         <v>0.63402777777777797</v>
       </c>
-      <c r="P49" s="13" t="str">
+      <c r="P49" s="17" t="str">
         <f t="shared" si="1"/>
         <v>133</v>
       </c>
-      <c r="U49" s="24" t="s">
+      <c r="U49" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="V49" s="24">
+      <c r="V49" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A50" s="7">
+      <c r="A50" s="16">
         <v>43197</v>
       </c>
       <c r="B50" s="1">
@@ -3780,115 +3809,129 @@
         <f t="shared" si="2"/>
         <v>0.24099999999999966</v>
       </c>
-      <c r="N50" s="13">
+      <c r="N50" s="17">
         <v>0.54236111111111096</v>
       </c>
-      <c r="O50" s="13">
+      <c r="O50" s="17">
         <v>0.63472222222222197</v>
       </c>
-      <c r="P50" s="13" t="str">
+      <c r="P50" s="17" t="str">
         <f t="shared" si="1"/>
         <v>133</v>
       </c>
-      <c r="U50" s="24" t="s">
+      <c r="U50" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="V50" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="8">
+      <c r="V50" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="18">
         <v>43197</v>
       </c>
-      <c r="B51" s="9">
-        <v>1</v>
-      </c>
-      <c r="C51" s="9">
-        <v>1</v>
-      </c>
-      <c r="D51" s="9">
+      <c r="B51" s="5">
+        <v>1</v>
+      </c>
+      <c r="C51" s="5">
+        <v>1</v>
+      </c>
+      <c r="D51" s="5">
         <v>2</v>
       </c>
-      <c r="E51" s="9" t="s">
+      <c r="E51" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F51" s="9">
+      <c r="F51" s="5">
         <v>25</v>
       </c>
-      <c r="G51" s="9">
+      <c r="G51" s="5">
         <v>29</v>
       </c>
-      <c r="H51" s="10">
-        <v>1</v>
-      </c>
-      <c r="I51" s="10">
+      <c r="H51" s="6">
+        <v>1</v>
+      </c>
+      <c r="I51" s="2">
         <v>34</v>
       </c>
-      <c r="J51" s="10">
+      <c r="J51" s="6">
         <v>23.9</v>
       </c>
-      <c r="K51" s="10">
+      <c r="K51" s="6">
         <v>17.239000000000001</v>
       </c>
-      <c r="L51" s="10">
+      <c r="L51" s="6">
         <v>17.459</v>
       </c>
-      <c r="M51" s="10">
+      <c r="M51" s="6">
         <f t="shared" si="2"/>
         <v>0.21999999999999886</v>
       </c>
-      <c r="N51" s="15">
+      <c r="N51" s="19">
         <v>0.54305555555555596</v>
       </c>
-      <c r="O51" s="15">
+      <c r="O51" s="19">
         <v>0.63541666666666696</v>
       </c>
-      <c r="P51" s="15" t="str">
+      <c r="P51" s="19" t="str">
         <f t="shared" si="1"/>
         <v>133</v>
       </c>
-      <c r="U51" s="12" t="s">
+      <c r="U51" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="V51" s="12">
+      <c r="V51" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:22" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="4">
+    <row r="52" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="14">
         <v>43198</v>
       </c>
-      <c r="B52" s="5">
-        <v>1</v>
-      </c>
-      <c r="C52" s="5">
-        <v>1</v>
-      </c>
-      <c r="D52" s="5">
-        <v>1</v>
-      </c>
-      <c r="E52" s="5" t="s">
+      <c r="B52" s="3">
+        <v>1</v>
+      </c>
+      <c r="C52" s="3">
+        <v>1</v>
+      </c>
+      <c r="D52" s="3">
+        <v>1</v>
+      </c>
+      <c r="E52" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F52" s="5">
-        <v>1</v>
-      </c>
-      <c r="G52" s="5">
+      <c r="F52" s="3">
+        <v>1</v>
+      </c>
+      <c r="G52" s="3">
         <v>29</v>
       </c>
-      <c r="H52" s="6">
-        <v>1</v>
-      </c>
-      <c r="I52" s="6"/>
-      <c r="J52" s="6"/>
-      <c r="P52" s="14" t="str">
+      <c r="H52" s="4">
+        <v>1</v>
+      </c>
+      <c r="I52" s="21">
+        <v>24</v>
+      </c>
+      <c r="J52" s="4">
+        <v>23.9</v>
+      </c>
+      <c r="K52" s="3">
+        <v>17.225999999999999</v>
+      </c>
+      <c r="L52" s="3">
+        <v>17.29</v>
+      </c>
+      <c r="M52" s="3">
+        <f t="shared" si="2"/>
+        <v>6.4000000000000057E-2</v>
+      </c>
+      <c r="P52" s="15" t="str">
         <f t="shared" si="1"/>
         <v>00</v>
       </c>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A53" s="7">
+      <c r="A53" s="16">
         <v>43198</v>
       </c>
       <c r="B53" s="1">
@@ -3912,15 +3955,29 @@
       <c r="H53" s="2">
         <v>1</v>
       </c>
-      <c r="I53" s="2"/>
-      <c r="J53" s="2"/>
-      <c r="P53" s="13" t="str">
+      <c r="I53" s="2">
+        <v>24</v>
+      </c>
+      <c r="J53" s="2">
+        <v>24.4</v>
+      </c>
+      <c r="K53" s="2">
+        <v>17.058</v>
+      </c>
+      <c r="L53" s="1">
+        <v>17.248000000000001</v>
+      </c>
+      <c r="M53" s="1">
+        <f t="shared" si="2"/>
+        <v>0.19000000000000128</v>
+      </c>
+      <c r="P53" s="17" t="str">
         <f t="shared" si="1"/>
         <v>00</v>
       </c>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A54" s="7">
+      <c r="A54" s="16">
         <v>43198</v>
       </c>
       <c r="B54" s="1">
@@ -3944,15 +4001,29 @@
       <c r="H54" s="2">
         <v>1</v>
       </c>
-      <c r="I54" s="2"/>
-      <c r="J54" s="2"/>
-      <c r="P54" s="13" t="str">
+      <c r="I54" s="2">
+        <v>24</v>
+      </c>
+      <c r="J54" s="2">
+        <v>25</v>
+      </c>
+      <c r="K54" s="2">
+        <v>17.146999999999998</v>
+      </c>
+      <c r="L54" s="1">
+        <v>17.215</v>
+      </c>
+      <c r="M54" s="1">
+        <f t="shared" si="2"/>
+        <v>6.8000000000001393E-2</v>
+      </c>
+      <c r="P54" s="17" t="str">
         <f t="shared" si="1"/>
         <v>00</v>
       </c>
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A55" s="7">
+      <c r="A55" s="16">
         <v>43198</v>
       </c>
       <c r="B55" s="1">
@@ -3976,15 +4047,29 @@
       <c r="H55" s="2">
         <v>1</v>
       </c>
-      <c r="I55" s="2"/>
-      <c r="J55" s="2"/>
-      <c r="P55" s="13" t="str">
+      <c r="I55" s="2">
+        <v>24</v>
+      </c>
+      <c r="J55" s="2">
+        <v>24.4</v>
+      </c>
+      <c r="K55" s="2">
+        <v>17.103999999999999</v>
+      </c>
+      <c r="L55" s="1">
+        <v>17.236000000000001</v>
+      </c>
+      <c r="M55" s="1">
+        <f t="shared" si="2"/>
+        <v>0.13200000000000145</v>
+      </c>
+      <c r="P55" s="17" t="str">
         <f t="shared" si="1"/>
         <v>00</v>
       </c>
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A56" s="7">
+      <c r="A56" s="16">
         <v>43198</v>
       </c>
       <c r="B56" s="1">
@@ -4008,15 +4093,29 @@
       <c r="H56" s="2">
         <v>1</v>
       </c>
-      <c r="I56" s="2"/>
-      <c r="J56" s="2"/>
-      <c r="P56" s="13" t="str">
+      <c r="I56" s="2">
+        <v>24</v>
+      </c>
+      <c r="J56" s="2">
+        <v>25</v>
+      </c>
+      <c r="K56" s="2">
+        <v>17.146999999999998</v>
+      </c>
+      <c r="L56" s="1">
+        <v>17.271999999999998</v>
+      </c>
+      <c r="M56" s="1">
+        <f t="shared" si="2"/>
+        <v>0.125</v>
+      </c>
+      <c r="P56" s="17" t="str">
         <f t="shared" si="1"/>
         <v>00</v>
       </c>
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A57" s="7">
+      <c r="A57" s="16">
         <v>43198</v>
       </c>
       <c r="B57" s="1">
@@ -4040,15 +4139,29 @@
       <c r="H57" s="2">
         <v>1</v>
       </c>
-      <c r="I57" s="2"/>
-      <c r="J57" s="2"/>
-      <c r="P57" s="13" t="str">
+      <c r="I57" s="2">
+        <v>24</v>
+      </c>
+      <c r="J57" s="2">
+        <v>25</v>
+      </c>
+      <c r="K57" s="2">
+        <v>17.253</v>
+      </c>
+      <c r="L57" s="1">
+        <v>17.372</v>
+      </c>
+      <c r="M57" s="1">
+        <f t="shared" si="2"/>
+        <v>0.11899999999999977</v>
+      </c>
+      <c r="P57" s="17" t="str">
         <f t="shared" si="1"/>
         <v>00</v>
       </c>
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A58" s="7">
+      <c r="A58" s="16">
         <v>43198</v>
       </c>
       <c r="B58" s="1">
@@ -4072,15 +4185,29 @@
       <c r="H58" s="2">
         <v>1</v>
       </c>
-      <c r="I58" s="2"/>
-      <c r="J58" s="2"/>
-      <c r="P58" s="13" t="str">
+      <c r="I58" s="2">
+        <v>24</v>
+      </c>
+      <c r="J58" s="2">
+        <v>24.3</v>
+      </c>
+      <c r="K58" s="2">
+        <v>16.844999999999999</v>
+      </c>
+      <c r="L58" s="1">
+        <v>16.998999999999999</v>
+      </c>
+      <c r="M58" s="1">
+        <f t="shared" si="2"/>
+        <v>0.15399999999999991</v>
+      </c>
+      <c r="P58" s="17" t="str">
         <f t="shared" si="1"/>
         <v>00</v>
       </c>
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A59" s="7">
+      <c r="A59" s="16">
         <v>43198</v>
       </c>
       <c r="B59" s="1">
@@ -4104,15 +4231,29 @@
       <c r="H59" s="2">
         <v>1</v>
       </c>
-      <c r="I59" s="2"/>
-      <c r="J59" s="2"/>
-      <c r="P59" s="13" t="str">
+      <c r="I59" s="2">
+        <v>24</v>
+      </c>
+      <c r="J59" s="2">
+        <v>24.3</v>
+      </c>
+      <c r="K59" s="2">
+        <v>16.913</v>
+      </c>
+      <c r="L59" s="1">
+        <v>17.016999999999999</v>
+      </c>
+      <c r="M59" s="1">
+        <f t="shared" si="2"/>
+        <v>0.1039999999999992</v>
+      </c>
+      <c r="P59" s="17" t="str">
         <f t="shared" si="1"/>
         <v>00</v>
       </c>
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A60" s="7">
+      <c r="A60" s="16">
         <v>43198</v>
       </c>
       <c r="B60" s="1">
@@ -4136,15 +4277,29 @@
       <c r="H60" s="2">
         <v>1</v>
       </c>
-      <c r="I60" s="2"/>
-      <c r="J60" s="2"/>
-      <c r="P60" s="13" t="str">
+      <c r="I60" s="2">
+        <v>24</v>
+      </c>
+      <c r="J60" s="2">
+        <v>24.6</v>
+      </c>
+      <c r="K60" s="2">
+        <v>17.451000000000001</v>
+      </c>
+      <c r="L60" s="1">
+        <v>17.439</v>
+      </c>
+      <c r="M60" s="1">
+        <f t="shared" si="2"/>
+        <v>-1.2000000000000455E-2</v>
+      </c>
+      <c r="P60" s="17" t="str">
         <f t="shared" si="1"/>
         <v>00</v>
       </c>
     </row>
     <row r="61" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A61" s="7">
+      <c r="A61" s="16">
         <v>43198</v>
       </c>
       <c r="B61" s="1">
@@ -4168,15 +4323,29 @@
       <c r="H61" s="2">
         <v>1</v>
       </c>
-      <c r="I61" s="2"/>
-      <c r="J61" s="2"/>
-      <c r="P61" s="13" t="str">
+      <c r="I61" s="2">
+        <v>24</v>
+      </c>
+      <c r="J61" s="2">
+        <v>23.9</v>
+      </c>
+      <c r="K61" s="2">
+        <v>17.337</v>
+      </c>
+      <c r="L61" s="1">
+        <v>17.452999999999999</v>
+      </c>
+      <c r="M61" s="1">
+        <f t="shared" si="2"/>
+        <v>0.11599999999999966</v>
+      </c>
+      <c r="P61" s="17" t="str">
         <f t="shared" si="1"/>
         <v>00</v>
       </c>
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A62" s="7">
+      <c r="A62" s="16">
         <v>43198</v>
       </c>
       <c r="B62" s="1">
@@ -4200,79 +4369,121 @@
       <c r="H62" s="2">
         <v>1</v>
       </c>
-      <c r="I62" s="2"/>
-      <c r="J62" s="2"/>
-      <c r="P62" s="13" t="str">
+      <c r="I62" s="2">
+        <v>24</v>
+      </c>
+      <c r="J62" s="2">
+        <v>25.6</v>
+      </c>
+      <c r="K62" s="2">
+        <v>17.212</v>
+      </c>
+      <c r="L62" s="1">
+        <v>17.364999999999998</v>
+      </c>
+      <c r="M62" s="1">
+        <f t="shared" si="2"/>
+        <v>0.15299999999999869</v>
+      </c>
+      <c r="P62" s="17" t="str">
         <f t="shared" si="1"/>
         <v>00</v>
       </c>
     </row>
-    <row r="63" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="8">
+    <row r="63" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="18">
         <v>43198</v>
       </c>
-      <c r="B63" s="9">
-        <v>1</v>
-      </c>
-      <c r="C63" s="9">
-        <v>1</v>
-      </c>
-      <c r="D63" s="9">
-        <v>1</v>
-      </c>
-      <c r="E63" s="9" t="s">
+      <c r="B63" s="5">
+        <v>1</v>
+      </c>
+      <c r="C63" s="5">
+        <v>1</v>
+      </c>
+      <c r="D63" s="5">
+        <v>1</v>
+      </c>
+      <c r="E63" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F63" s="9">
+      <c r="F63" s="5">
         <v>12</v>
       </c>
-      <c r="G63" s="9">
+      <c r="G63" s="5">
         <v>23</v>
       </c>
-      <c r="H63" s="10">
-        <v>1</v>
-      </c>
-      <c r="I63" s="10"/>
-      <c r="J63" s="10"/>
-      <c r="P63" s="15" t="str">
+      <c r="H63" s="6">
+        <v>1</v>
+      </c>
+      <c r="I63" s="2">
+        <v>24</v>
+      </c>
+      <c r="J63" s="6">
+        <v>24.2</v>
+      </c>
+      <c r="K63" s="5">
+        <v>16.786999999999999</v>
+      </c>
+      <c r="L63" s="5">
+        <v>16.852</v>
+      </c>
+      <c r="M63" s="5">
+        <f t="shared" si="2"/>
+        <v>6.5000000000001279E-2</v>
+      </c>
+      <c r="P63" s="19" t="str">
         <f t="shared" si="1"/>
         <v>00</v>
       </c>
     </row>
-    <row r="64" spans="1:22" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="4">
+    <row r="64" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="14">
         <v>43198</v>
       </c>
-      <c r="B64" s="5">
-        <v>1</v>
-      </c>
-      <c r="C64" s="5">
-        <v>1</v>
-      </c>
-      <c r="D64" s="5">
+      <c r="B64" s="3">
+        <v>1</v>
+      </c>
+      <c r="C64" s="3">
+        <v>1</v>
+      </c>
+      <c r="D64" s="3">
         <v>2</v>
       </c>
-      <c r="E64" s="5" t="s">
+      <c r="E64" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F64" s="5">
+      <c r="F64" s="3">
         <v>13</v>
       </c>
-      <c r="G64" s="5">
+      <c r="G64" s="3">
         <v>23</v>
       </c>
-      <c r="H64" s="6">
-        <v>1</v>
-      </c>
-      <c r="I64" s="6"/>
-      <c r="J64" s="6"/>
-      <c r="P64" s="14" t="str">
+      <c r="H64" s="4">
+        <v>1</v>
+      </c>
+      <c r="I64" s="21">
+        <v>32</v>
+      </c>
+      <c r="J64" s="4">
+        <v>24.6</v>
+      </c>
+      <c r="K64" s="3">
+        <v>17.263000000000002</v>
+      </c>
+      <c r="L64" s="3">
+        <v>17.335000000000001</v>
+      </c>
+      <c r="M64" s="3">
+        <f t="shared" si="2"/>
+        <v>7.1999999999999176E-2</v>
+      </c>
+      <c r="P64" s="15" t="str">
         <f t="shared" si="1"/>
         <v>00</v>
       </c>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A65" s="7">
+      <c r="A65" s="16">
         <v>43198</v>
       </c>
       <c r="B65" s="1">
@@ -4296,15 +4507,29 @@
       <c r="H65" s="2">
         <v>1</v>
       </c>
-      <c r="I65" s="2"/>
-      <c r="J65" s="2"/>
-      <c r="P65" s="13" t="str">
+      <c r="I65" s="2">
+        <v>32</v>
+      </c>
+      <c r="J65" s="2">
+        <v>25</v>
+      </c>
+      <c r="K65" s="1">
+        <v>17.196000000000002</v>
+      </c>
+      <c r="L65" s="1">
+        <v>17.289000000000001</v>
+      </c>
+      <c r="M65" s="1">
+        <f t="shared" si="2"/>
+        <v>9.2999999999999972E-2</v>
+      </c>
+      <c r="P65" s="17" t="str">
         <f t="shared" si="1"/>
         <v>00</v>
       </c>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A66" s="7">
+      <c r="A66" s="16">
         <v>43198</v>
       </c>
       <c r="B66" s="1">
@@ -4328,15 +4553,29 @@
       <c r="H66" s="2">
         <v>1</v>
       </c>
-      <c r="I66" s="2"/>
-      <c r="J66" s="2"/>
-      <c r="P66" s="13" t="str">
+      <c r="I66" s="2">
+        <v>32</v>
+      </c>
+      <c r="J66" s="2">
+        <v>24.4</v>
+      </c>
+      <c r="K66" s="1">
+        <v>16.919</v>
+      </c>
+      <c r="L66" s="1">
+        <v>17.042000000000002</v>
+      </c>
+      <c r="M66" s="1">
+        <f t="shared" si="2"/>
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="P66" s="17" t="str">
         <f t="shared" si="1"/>
         <v>00</v>
       </c>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A67" s="7">
+      <c r="A67" s="16">
         <v>43198</v>
       </c>
       <c r="B67" s="1">
@@ -4360,15 +4599,29 @@
       <c r="H67" s="2">
         <v>1</v>
       </c>
-      <c r="I67" s="2"/>
-      <c r="J67" s="2"/>
-      <c r="P67" s="13" t="str">
+      <c r="I67" s="2">
+        <v>32</v>
+      </c>
+      <c r="J67" s="2">
+        <v>24.4</v>
+      </c>
+      <c r="K67" s="1">
+        <v>17.350999999999999</v>
+      </c>
+      <c r="L67" s="1">
+        <v>17.503</v>
+      </c>
+      <c r="M67" s="1">
+        <f t="shared" si="2"/>
+        <v>0.15200000000000102</v>
+      </c>
+      <c r="P67" s="17" t="str">
         <f t="shared" ref="P67:P101" si="3">TEXT(O67-N67, "[mm]")</f>
         <v>00</v>
       </c>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A68" s="7">
+      <c r="A68" s="16">
         <v>43198</v>
       </c>
       <c r="B68" s="1">
@@ -4392,15 +4645,29 @@
       <c r="H68" s="2">
         <v>1</v>
       </c>
-      <c r="I68" s="2"/>
-      <c r="J68" s="2"/>
-      <c r="P68" s="13" t="str">
+      <c r="I68" s="2">
+        <v>32</v>
+      </c>
+      <c r="J68" s="2">
+        <v>25.5</v>
+      </c>
+      <c r="K68" s="1">
+        <v>17.242999999999999</v>
+      </c>
+      <c r="L68" s="1">
+        <v>17.364000000000001</v>
+      </c>
+      <c r="M68" s="1">
+        <f t="shared" si="2"/>
+        <v>0.12100000000000222</v>
+      </c>
+      <c r="P68" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00</v>
       </c>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A69" s="7">
+      <c r="A69" s="16">
         <v>43198</v>
       </c>
       <c r="B69" s="1">
@@ -4424,15 +4691,29 @@
       <c r="H69" s="2">
         <v>1</v>
       </c>
-      <c r="I69" s="2"/>
-      <c r="J69" s="2"/>
-      <c r="P69" s="13" t="str">
+      <c r="I69" s="2">
+        <v>32</v>
+      </c>
+      <c r="J69" s="2">
+        <v>23.5</v>
+      </c>
+      <c r="K69" s="1">
+        <v>17.213999999999999</v>
+      </c>
+      <c r="L69" s="1">
+        <v>17.350000000000001</v>
+      </c>
+      <c r="M69" s="1">
+        <f t="shared" si="2"/>
+        <v>0.13600000000000279</v>
+      </c>
+      <c r="P69" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00</v>
       </c>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A70" s="7">
+      <c r="A70" s="16">
         <v>43198</v>
       </c>
       <c r="B70" s="1">
@@ -4456,15 +4737,29 @@
       <c r="H70" s="2">
         <v>1</v>
       </c>
-      <c r="I70" s="2"/>
-      <c r="J70" s="2"/>
-      <c r="P70" s="13" t="str">
+      <c r="I70" s="2">
+        <v>32</v>
+      </c>
+      <c r="J70" s="2">
+        <v>24.4</v>
+      </c>
+      <c r="K70" s="1">
+        <v>17.027999999999999</v>
+      </c>
+      <c r="L70" s="1">
+        <v>17.137</v>
+      </c>
+      <c r="M70" s="1">
+        <f t="shared" si="2"/>
+        <v>0.10900000000000176</v>
+      </c>
+      <c r="P70" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00</v>
       </c>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A71" s="7">
+      <c r="A71" s="16">
         <v>43198</v>
       </c>
       <c r="B71" s="1">
@@ -4488,15 +4783,29 @@
       <c r="H71" s="2">
         <v>1</v>
       </c>
-      <c r="I71" s="2"/>
-      <c r="J71" s="2"/>
-      <c r="P71" s="13" t="str">
+      <c r="I71" s="2">
+        <v>32</v>
+      </c>
+      <c r="J71" s="2">
+        <v>25.1</v>
+      </c>
+      <c r="K71" s="1">
+        <v>16.981000000000002</v>
+      </c>
+      <c r="L71" s="1">
+        <v>17.117999999999999</v>
+      </c>
+      <c r="M71" s="1">
+        <f t="shared" si="2"/>
+        <v>0.1369999999999969</v>
+      </c>
+      <c r="P71" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00</v>
       </c>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A72" s="7">
+      <c r="A72" s="16">
         <v>43198</v>
       </c>
       <c r="B72" s="1">
@@ -4520,15 +4829,29 @@
       <c r="H72" s="2">
         <v>1</v>
       </c>
-      <c r="I72" s="2"/>
-      <c r="J72" s="2"/>
-      <c r="P72" s="13" t="str">
+      <c r="I72" s="2">
+        <v>32</v>
+      </c>
+      <c r="J72" s="2">
+        <v>24.2</v>
+      </c>
+      <c r="K72" s="1">
+        <v>17.123000000000001</v>
+      </c>
+      <c r="L72" s="1">
+        <v>17.335000000000001</v>
+      </c>
+      <c r="M72" s="1">
+        <f t="shared" si="2"/>
+        <v>0.21199999999999974</v>
+      </c>
+      <c r="P72" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00</v>
       </c>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A73" s="7">
+      <c r="A73" s="16">
         <v>43198</v>
       </c>
       <c r="B73" s="1">
@@ -4552,15 +4875,29 @@
       <c r="H73" s="2">
         <v>1</v>
       </c>
-      <c r="I73" s="2"/>
-      <c r="J73" s="2"/>
-      <c r="P73" s="13" t="str">
+      <c r="I73" s="2">
+        <v>32</v>
+      </c>
+      <c r="J73" s="2">
+        <v>24.4</v>
+      </c>
+      <c r="K73" s="1">
+        <v>17.440999999999999</v>
+      </c>
+      <c r="L73" s="1">
+        <v>17.617999999999999</v>
+      </c>
+      <c r="M73" s="1">
+        <f t="shared" si="2"/>
+        <v>0.1769999999999996</v>
+      </c>
+      <c r="P73" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00</v>
       </c>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A74" s="7">
+      <c r="A74" s="16">
         <v>43198</v>
       </c>
       <c r="B74" s="1">
@@ -4584,15 +4921,29 @@
       <c r="H74" s="2">
         <v>1</v>
       </c>
-      <c r="I74" s="2"/>
-      <c r="J74" s="2"/>
-      <c r="P74" s="13" t="str">
+      <c r="I74" s="2">
+        <v>32</v>
+      </c>
+      <c r="J74" s="2">
+        <v>24.8</v>
+      </c>
+      <c r="K74" s="1">
+        <v>17.420000000000002</v>
+      </c>
+      <c r="L74" s="1">
+        <v>17.576000000000001</v>
+      </c>
+      <c r="M74" s="1">
+        <f t="shared" si="2"/>
+        <v>0.15599999999999881</v>
+      </c>
+      <c r="P74" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00</v>
       </c>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A75" s="7">
+      <c r="A75" s="16">
         <v>43198</v>
       </c>
       <c r="B75" s="1">
@@ -4616,79 +4967,121 @@
       <c r="H75" s="2">
         <v>1</v>
       </c>
-      <c r="I75" s="2"/>
-      <c r="J75" s="2"/>
-      <c r="P75" s="13" t="str">
+      <c r="I75" s="2">
+        <v>32</v>
+      </c>
+      <c r="J75" s="2">
+        <v>24.8</v>
+      </c>
+      <c r="K75" s="1">
+        <v>17.446000000000002</v>
+      </c>
+      <c r="L75" s="1">
+        <v>17.568999999999999</v>
+      </c>
+      <c r="M75" s="1">
+        <f t="shared" si="2"/>
+        <v>0.12299999999999756</v>
+      </c>
+      <c r="P75" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00</v>
       </c>
     </row>
-    <row r="76" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="8">
+    <row r="76" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="18">
         <v>43198</v>
       </c>
-      <c r="B76" s="9">
-        <v>1</v>
-      </c>
-      <c r="C76" s="9">
-        <v>1</v>
-      </c>
-      <c r="D76" s="9">
+      <c r="B76" s="5">
+        <v>1</v>
+      </c>
+      <c r="C76" s="5">
+        <v>1</v>
+      </c>
+      <c r="D76" s="5">
         <v>2</v>
       </c>
-      <c r="E76" s="9" t="s">
+      <c r="E76" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F76" s="9">
+      <c r="F76" s="5">
         <v>25</v>
       </c>
-      <c r="G76" s="9">
+      <c r="G76" s="5">
         <v>29</v>
       </c>
-      <c r="H76" s="10">
-        <v>1</v>
-      </c>
-      <c r="I76" s="10"/>
-      <c r="J76" s="10"/>
-      <c r="P76" s="15" t="str">
+      <c r="H76" s="6">
+        <v>1</v>
+      </c>
+      <c r="I76" s="2">
+        <v>32</v>
+      </c>
+      <c r="J76" s="2">
+        <v>25.2</v>
+      </c>
+      <c r="K76" s="5">
+        <v>17.178999999999998</v>
+      </c>
+      <c r="L76" s="5">
+        <v>17.32</v>
+      </c>
+      <c r="M76" s="5">
+        <f t="shared" si="2"/>
+        <v>0.14100000000000179</v>
+      </c>
+      <c r="P76" s="19" t="str">
         <f t="shared" si="3"/>
         <v>00</v>
       </c>
     </row>
-    <row r="77" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="4">
+    <row r="77" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="14">
         <v>43198</v>
       </c>
-      <c r="B77" s="5">
-        <v>1</v>
-      </c>
-      <c r="C77" s="5">
-        <v>1</v>
-      </c>
-      <c r="D77" s="5">
-        <v>1</v>
-      </c>
-      <c r="E77" s="5" t="s">
+      <c r="B77" s="3">
+        <v>1</v>
+      </c>
+      <c r="C77" s="3">
+        <v>1</v>
+      </c>
+      <c r="D77" s="3">
+        <v>1</v>
+      </c>
+      <c r="E77" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F77" s="5">
-        <v>1</v>
-      </c>
-      <c r="G77" s="5">
+      <c r="F77" s="3">
+        <v>1</v>
+      </c>
+      <c r="G77" s="3">
         <v>29</v>
       </c>
-      <c r="H77" s="6">
-        <v>1</v>
-      </c>
-      <c r="I77" s="6"/>
-      <c r="J77" s="6"/>
-      <c r="P77" s="14" t="str">
+      <c r="H77" s="4">
+        <v>1</v>
+      </c>
+      <c r="I77" s="21">
+        <v>32</v>
+      </c>
+      <c r="J77" s="4">
+        <v>23.9</v>
+      </c>
+      <c r="K77" s="3">
+        <v>17.225999999999999</v>
+      </c>
+      <c r="L77" s="3">
+        <v>17.29</v>
+      </c>
+      <c r="M77" s="3">
+        <f t="shared" ref="M77:M101" si="4">L77-K77</f>
+        <v>6.4000000000000057E-2</v>
+      </c>
+      <c r="P77" s="15" t="str">
         <f t="shared" si="3"/>
         <v>00</v>
       </c>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A78" s="7">
+      <c r="A78" s="16">
         <v>43198</v>
       </c>
       <c r="B78" s="1">
@@ -4712,15 +5105,29 @@
       <c r="H78" s="2">
         <v>1</v>
       </c>
-      <c r="I78" s="2"/>
-      <c r="J78" s="2"/>
-      <c r="P78" s="13" t="str">
+      <c r="I78" s="2">
+        <v>32</v>
+      </c>
+      <c r="J78" s="2">
+        <v>24.4</v>
+      </c>
+      <c r="K78" s="2">
+        <v>17.058</v>
+      </c>
+      <c r="L78" s="1">
+        <v>17.248000000000001</v>
+      </c>
+      <c r="M78" s="1">
+        <f t="shared" si="4"/>
+        <v>0.19000000000000128</v>
+      </c>
+      <c r="P78" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00</v>
       </c>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A79" s="7">
+      <c r="A79" s="16">
         <v>43198</v>
       </c>
       <c r="B79" s="1">
@@ -4744,15 +5151,29 @@
       <c r="H79" s="2">
         <v>1</v>
       </c>
-      <c r="I79" s="2"/>
-      <c r="J79" s="2"/>
-      <c r="P79" s="13" t="str">
+      <c r="I79" s="2">
+        <v>32</v>
+      </c>
+      <c r="J79" s="2">
+        <v>25</v>
+      </c>
+      <c r="K79" s="2">
+        <v>17.146999999999998</v>
+      </c>
+      <c r="L79" s="1">
+        <v>17.215</v>
+      </c>
+      <c r="M79" s="1">
+        <f t="shared" si="4"/>
+        <v>6.8000000000001393E-2</v>
+      </c>
+      <c r="P79" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00</v>
       </c>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A80" s="7">
+      <c r="A80" s="16">
         <v>43198</v>
       </c>
       <c r="B80" s="1">
@@ -4776,15 +5197,29 @@
       <c r="H80" s="2">
         <v>1</v>
       </c>
-      <c r="I80" s="2"/>
-      <c r="J80" s="2"/>
-      <c r="P80" s="13" t="str">
+      <c r="I80" s="2">
+        <v>32</v>
+      </c>
+      <c r="J80" s="2">
+        <v>24.4</v>
+      </c>
+      <c r="K80" s="2">
+        <v>17.103999999999999</v>
+      </c>
+      <c r="L80" s="1">
+        <v>17.236000000000001</v>
+      </c>
+      <c r="M80" s="1">
+        <f t="shared" si="4"/>
+        <v>0.13200000000000145</v>
+      </c>
+      <c r="P80" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00</v>
       </c>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A81" s="7">
+      <c r="A81" s="16">
         <v>43198</v>
       </c>
       <c r="B81" s="1">
@@ -4808,15 +5243,29 @@
       <c r="H81" s="2">
         <v>1</v>
       </c>
-      <c r="I81" s="2"/>
-      <c r="J81" s="2"/>
-      <c r="P81" s="13" t="str">
+      <c r="I81" s="2">
+        <v>32</v>
+      </c>
+      <c r="J81" s="2">
+        <v>25</v>
+      </c>
+      <c r="K81" s="2">
+        <v>17.146999999999998</v>
+      </c>
+      <c r="L81" s="1">
+        <v>17.271999999999998</v>
+      </c>
+      <c r="M81" s="1">
+        <f t="shared" si="4"/>
+        <v>0.125</v>
+      </c>
+      <c r="P81" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00</v>
       </c>
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A82" s="7">
+      <c r="A82" s="16">
         <v>43198</v>
       </c>
       <c r="B82" s="1">
@@ -4840,15 +5289,29 @@
       <c r="H82" s="2">
         <v>1</v>
       </c>
-      <c r="I82" s="2"/>
-      <c r="J82" s="2"/>
-      <c r="P82" s="13" t="str">
+      <c r="I82" s="2">
+        <v>32</v>
+      </c>
+      <c r="J82" s="2">
+        <v>25</v>
+      </c>
+      <c r="K82" s="2">
+        <v>17.253</v>
+      </c>
+      <c r="L82" s="1">
+        <v>17.372</v>
+      </c>
+      <c r="M82" s="1">
+        <f t="shared" si="4"/>
+        <v>0.11899999999999977</v>
+      </c>
+      <c r="P82" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00</v>
       </c>
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A83" s="7">
+      <c r="A83" s="16">
         <v>43198</v>
       </c>
       <c r="B83" s="1">
@@ -4872,15 +5335,29 @@
       <c r="H83" s="2">
         <v>1</v>
       </c>
-      <c r="I83" s="2"/>
-      <c r="J83" s="2"/>
-      <c r="P83" s="13" t="str">
+      <c r="I83" s="2">
+        <v>32</v>
+      </c>
+      <c r="J83" s="2">
+        <v>24.3</v>
+      </c>
+      <c r="K83" s="2">
+        <v>16.844999999999999</v>
+      </c>
+      <c r="L83" s="1">
+        <v>16.998999999999999</v>
+      </c>
+      <c r="M83" s="1">
+        <f t="shared" si="4"/>
+        <v>0.15399999999999991</v>
+      </c>
+      <c r="P83" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00</v>
       </c>
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A84" s="7">
+      <c r="A84" s="16">
         <v>43198</v>
       </c>
       <c r="B84" s="1">
@@ -4904,15 +5381,29 @@
       <c r="H84" s="2">
         <v>1</v>
       </c>
-      <c r="I84" s="2"/>
-      <c r="J84" s="2"/>
-      <c r="P84" s="13" t="str">
+      <c r="I84" s="2">
+        <v>32</v>
+      </c>
+      <c r="J84" s="2">
+        <v>24.3</v>
+      </c>
+      <c r="K84" s="2">
+        <v>16.913</v>
+      </c>
+      <c r="L84" s="1">
+        <v>17.016999999999999</v>
+      </c>
+      <c r="M84" s="1">
+        <f t="shared" si="4"/>
+        <v>0.1039999999999992</v>
+      </c>
+      <c r="P84" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00</v>
       </c>
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A85" s="7">
+      <c r="A85" s="16">
         <v>43198</v>
       </c>
       <c r="B85" s="1">
@@ -4936,15 +5427,29 @@
       <c r="H85" s="2">
         <v>1</v>
       </c>
-      <c r="I85" s="2"/>
-      <c r="J85" s="2"/>
-      <c r="P85" s="13" t="str">
+      <c r="I85" s="2">
+        <v>32</v>
+      </c>
+      <c r="J85" s="2">
+        <v>24.6</v>
+      </c>
+      <c r="K85" s="2">
+        <v>17.451000000000001</v>
+      </c>
+      <c r="L85" s="1">
+        <v>17.439</v>
+      </c>
+      <c r="M85" s="1">
+        <f t="shared" si="4"/>
+        <v>-1.2000000000000455E-2</v>
+      </c>
+      <c r="P85" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00</v>
       </c>
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A86" s="7">
+      <c r="A86" s="16">
         <v>43198</v>
       </c>
       <c r="B86" s="1">
@@ -4968,15 +5473,29 @@
       <c r="H86" s="2">
         <v>1</v>
       </c>
-      <c r="I86" s="2"/>
-      <c r="J86" s="2"/>
-      <c r="P86" s="13" t="str">
+      <c r="I86" s="2">
+        <v>32</v>
+      </c>
+      <c r="J86" s="2">
+        <v>23.9</v>
+      </c>
+      <c r="K86" s="2">
+        <v>17.337</v>
+      </c>
+      <c r="L86" s="1">
+        <v>17.452999999999999</v>
+      </c>
+      <c r="M86" s="1">
+        <f t="shared" si="4"/>
+        <v>0.11599999999999966</v>
+      </c>
+      <c r="P86" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00</v>
       </c>
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A87" s="7">
+      <c r="A87" s="16">
         <v>43198</v>
       </c>
       <c r="B87" s="1">
@@ -5000,79 +5519,121 @@
       <c r="H87" s="2">
         <v>1</v>
       </c>
-      <c r="I87" s="2"/>
-      <c r="J87" s="2"/>
-      <c r="P87" s="13" t="str">
+      <c r="I87" s="2">
+        <v>32</v>
+      </c>
+      <c r="J87" s="2">
+        <v>25.6</v>
+      </c>
+      <c r="K87" s="2">
+        <v>17.212</v>
+      </c>
+      <c r="L87" s="1">
+        <v>17.364999999999998</v>
+      </c>
+      <c r="M87" s="1">
+        <f t="shared" si="4"/>
+        <v>0.15299999999999869</v>
+      </c>
+      <c r="P87" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00</v>
       </c>
     </row>
-    <row r="88" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="8">
+    <row r="88" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="18">
         <v>43198</v>
       </c>
-      <c r="B88" s="9">
-        <v>1</v>
-      </c>
-      <c r="C88" s="9">
-        <v>1</v>
-      </c>
-      <c r="D88" s="9">
-        <v>1</v>
-      </c>
-      <c r="E88" s="9" t="s">
+      <c r="B88" s="5">
+        <v>1</v>
+      </c>
+      <c r="C88" s="5">
+        <v>1</v>
+      </c>
+      <c r="D88" s="5">
+        <v>1</v>
+      </c>
+      <c r="E88" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F88" s="9">
+      <c r="F88" s="5">
         <v>12</v>
       </c>
-      <c r="G88" s="9">
+      <c r="G88" s="5">
         <v>23</v>
       </c>
-      <c r="H88" s="10">
-        <v>1</v>
-      </c>
-      <c r="I88" s="10"/>
-      <c r="J88" s="10"/>
-      <c r="P88" s="15" t="str">
+      <c r="H88" s="6">
+        <v>1</v>
+      </c>
+      <c r="I88" s="20">
+        <v>32</v>
+      </c>
+      <c r="J88" s="6">
+        <v>24.2</v>
+      </c>
+      <c r="K88" s="5">
+        <v>16.786999999999999</v>
+      </c>
+      <c r="L88" s="5">
+        <v>16.852</v>
+      </c>
+      <c r="M88" s="5">
+        <f t="shared" si="4"/>
+        <v>6.5000000000001279E-2</v>
+      </c>
+      <c r="P88" s="19" t="str">
         <f t="shared" si="3"/>
         <v>00</v>
       </c>
     </row>
-    <row r="89" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="4">
+    <row r="89" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="14">
         <v>43198</v>
       </c>
-      <c r="B89" s="5">
-        <v>1</v>
-      </c>
-      <c r="C89" s="5">
-        <v>1</v>
-      </c>
-      <c r="D89" s="5">
+      <c r="B89" s="3">
+        <v>1</v>
+      </c>
+      <c r="C89" s="3">
+        <v>1</v>
+      </c>
+      <c r="D89" s="3">
         <v>2</v>
       </c>
-      <c r="E89" s="5" t="s">
+      <c r="E89" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F89" s="5">
+      <c r="F89" s="3">
         <v>13</v>
       </c>
-      <c r="G89" s="5">
+      <c r="G89" s="3">
         <v>23</v>
       </c>
-      <c r="H89" s="6">
-        <v>1</v>
-      </c>
-      <c r="I89" s="6"/>
-      <c r="J89" s="6"/>
-      <c r="P89" s="14" t="str">
+      <c r="H89" s="4">
+        <v>1</v>
+      </c>
+      <c r="I89" s="2">
+        <v>28</v>
+      </c>
+      <c r="J89" s="4">
+        <v>24.6</v>
+      </c>
+      <c r="K89" s="3">
+        <v>17.263000000000002</v>
+      </c>
+      <c r="L89" s="3">
+        <v>17.335000000000001</v>
+      </c>
+      <c r="M89" s="3">
+        <f t="shared" si="4"/>
+        <v>7.1999999999999176E-2</v>
+      </c>
+      <c r="P89" s="15" t="str">
         <f t="shared" si="3"/>
         <v>00</v>
       </c>
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A90" s="7">
+      <c r="A90" s="16">
         <v>43198</v>
       </c>
       <c r="B90" s="1">
@@ -5096,15 +5657,29 @@
       <c r="H90" s="2">
         <v>1</v>
       </c>
-      <c r="I90" s="2"/>
-      <c r="J90" s="2"/>
-      <c r="P90" s="13" t="str">
+      <c r="I90" s="2">
+        <v>28</v>
+      </c>
+      <c r="J90" s="2">
+        <v>25</v>
+      </c>
+      <c r="K90" s="1">
+        <v>17.196000000000002</v>
+      </c>
+      <c r="L90" s="1">
+        <v>17.289000000000001</v>
+      </c>
+      <c r="M90" s="1">
+        <f t="shared" si="4"/>
+        <v>9.2999999999999972E-2</v>
+      </c>
+      <c r="P90" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00</v>
       </c>
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A91" s="7">
+      <c r="A91" s="16">
         <v>43198</v>
       </c>
       <c r="B91" s="1">
@@ -5128,15 +5703,29 @@
       <c r="H91" s="2">
         <v>1</v>
       </c>
-      <c r="I91" s="2"/>
-      <c r="J91" s="2"/>
-      <c r="P91" s="13" t="str">
+      <c r="I91" s="2">
+        <v>28</v>
+      </c>
+      <c r="J91" s="2">
+        <v>24.4</v>
+      </c>
+      <c r="K91" s="1">
+        <v>16.919</v>
+      </c>
+      <c r="L91" s="1">
+        <v>17.042000000000002</v>
+      </c>
+      <c r="M91" s="1">
+        <f t="shared" si="4"/>
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="P91" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00</v>
       </c>
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A92" s="7">
+      <c r="A92" s="16">
         <v>43198</v>
       </c>
       <c r="B92" s="1">
@@ -5160,15 +5749,29 @@
       <c r="H92" s="2">
         <v>1</v>
       </c>
-      <c r="I92" s="2"/>
-      <c r="J92" s="2"/>
-      <c r="P92" s="13" t="str">
+      <c r="I92" s="2">
+        <v>28</v>
+      </c>
+      <c r="J92" s="2">
+        <v>24.4</v>
+      </c>
+      <c r="K92" s="1">
+        <v>17.350999999999999</v>
+      </c>
+      <c r="L92" s="1">
+        <v>17.503</v>
+      </c>
+      <c r="M92" s="1">
+        <f t="shared" si="4"/>
+        <v>0.15200000000000102</v>
+      </c>
+      <c r="P92" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00</v>
       </c>
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A93" s="7">
+      <c r="A93" s="16">
         <v>43198</v>
       </c>
       <c r="B93" s="1">
@@ -5192,15 +5795,29 @@
       <c r="H93" s="2">
         <v>1</v>
       </c>
-      <c r="I93" s="2"/>
-      <c r="J93" s="2"/>
-      <c r="P93" s="13" t="str">
+      <c r="I93" s="2">
+        <v>28</v>
+      </c>
+      <c r="J93" s="2">
+        <v>25.5</v>
+      </c>
+      <c r="K93" s="1">
+        <v>17.242999999999999</v>
+      </c>
+      <c r="L93" s="1">
+        <v>17.364000000000001</v>
+      </c>
+      <c r="M93" s="1">
+        <f t="shared" si="4"/>
+        <v>0.12100000000000222</v>
+      </c>
+      <c r="P93" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00</v>
       </c>
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A94" s="7">
+      <c r="A94" s="16">
         <v>43198</v>
       </c>
       <c r="B94" s="1">
@@ -5224,15 +5841,29 @@
       <c r="H94" s="2">
         <v>1</v>
       </c>
-      <c r="I94" s="2"/>
-      <c r="J94" s="2"/>
-      <c r="P94" s="13" t="str">
+      <c r="I94" s="2">
+        <v>28</v>
+      </c>
+      <c r="J94" s="2">
+        <v>23.5</v>
+      </c>
+      <c r="K94" s="1">
+        <v>17.213999999999999</v>
+      </c>
+      <c r="L94" s="1">
+        <v>17.350000000000001</v>
+      </c>
+      <c r="M94" s="1">
+        <f t="shared" si="4"/>
+        <v>0.13600000000000279</v>
+      </c>
+      <c r="P94" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00</v>
       </c>
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A95" s="7">
+      <c r="A95" s="16">
         <v>43198</v>
       </c>
       <c r="B95" s="1">
@@ -5256,15 +5887,29 @@
       <c r="H95" s="2">
         <v>1</v>
       </c>
-      <c r="I95" s="2"/>
-      <c r="J95" s="2"/>
-      <c r="P95" s="13" t="str">
+      <c r="I95" s="2">
+        <v>28</v>
+      </c>
+      <c r="J95" s="2">
+        <v>24.4</v>
+      </c>
+      <c r="K95" s="1">
+        <v>17.027999999999999</v>
+      </c>
+      <c r="L95" s="1">
+        <v>17.137</v>
+      </c>
+      <c r="M95" s="1">
+        <f t="shared" si="4"/>
+        <v>0.10900000000000176</v>
+      </c>
+      <c r="P95" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00</v>
       </c>
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A96" s="7">
+      <c r="A96" s="16">
         <v>43198</v>
       </c>
       <c r="B96" s="1">
@@ -5288,14 +5933,29 @@
       <c r="H96" s="2">
         <v>1</v>
       </c>
-      <c r="J96" s="2"/>
-      <c r="P96" s="13" t="str">
+      <c r="I96" s="2">
+        <v>28</v>
+      </c>
+      <c r="J96" s="2">
+        <v>25.1</v>
+      </c>
+      <c r="K96" s="1">
+        <v>16.981000000000002</v>
+      </c>
+      <c r="L96" s="1">
+        <v>17.117999999999999</v>
+      </c>
+      <c r="M96" s="1">
+        <f t="shared" si="4"/>
+        <v>0.1369999999999969</v>
+      </c>
+      <c r="P96" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00</v>
       </c>
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A97" s="7">
+      <c r="A97" s="16">
         <v>43198</v>
       </c>
       <c r="B97" s="1">
@@ -5319,14 +5979,29 @@
       <c r="H97" s="2">
         <v>1</v>
       </c>
-      <c r="J97" s="2"/>
-      <c r="P97" s="13" t="str">
+      <c r="I97" s="2">
+        <v>28</v>
+      </c>
+      <c r="J97" s="2">
+        <v>24.2</v>
+      </c>
+      <c r="K97" s="1">
+        <v>17.123000000000001</v>
+      </c>
+      <c r="L97" s="1">
+        <v>17.335000000000001</v>
+      </c>
+      <c r="M97" s="1">
+        <f t="shared" si="4"/>
+        <v>0.21199999999999974</v>
+      </c>
+      <c r="P97" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00</v>
       </c>
     </row>
     <row r="98" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A98" s="7">
+      <c r="A98" s="16">
         <v>43198</v>
       </c>
       <c r="B98" s="1">
@@ -5350,14 +6025,29 @@
       <c r="H98" s="2">
         <v>1</v>
       </c>
-      <c r="J98" s="2"/>
-      <c r="P98" s="13" t="str">
+      <c r="I98" s="2">
+        <v>28</v>
+      </c>
+      <c r="J98" s="2">
+        <v>24.4</v>
+      </c>
+      <c r="K98" s="1">
+        <v>17.440999999999999</v>
+      </c>
+      <c r="L98" s="1">
+        <v>17.617999999999999</v>
+      </c>
+      <c r="M98" s="1">
+        <f t="shared" si="4"/>
+        <v>0.1769999999999996</v>
+      </c>
+      <c r="P98" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00</v>
       </c>
     </row>
     <row r="99" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A99" s="7">
+      <c r="A99" s="16">
         <v>43198</v>
       </c>
       <c r="B99" s="1">
@@ -5381,14 +6071,29 @@
       <c r="H99" s="2">
         <v>1</v>
       </c>
-      <c r="J99" s="2"/>
-      <c r="P99" s="13" t="str">
+      <c r="I99" s="2">
+        <v>28</v>
+      </c>
+      <c r="J99" s="2">
+        <v>24.8</v>
+      </c>
+      <c r="K99" s="1">
+        <v>17.420000000000002</v>
+      </c>
+      <c r="L99" s="1">
+        <v>17.576000000000001</v>
+      </c>
+      <c r="M99" s="1">
+        <f t="shared" si="4"/>
+        <v>0.15599999999999881</v>
+      </c>
+      <c r="P99" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00</v>
       </c>
     </row>
     <row r="100" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A100" s="7">
+      <c r="A100" s="16">
         <v>43198</v>
       </c>
       <c r="B100" s="1">
@@ -5412,46 +6117,76 @@
       <c r="H100" s="2">
         <v>1</v>
       </c>
-      <c r="J100" s="2"/>
-      <c r="P100" s="13" t="str">
+      <c r="I100" s="2">
+        <v>28</v>
+      </c>
+      <c r="J100" s="2">
+        <v>24.8</v>
+      </c>
+      <c r="K100" s="1">
+        <v>17.446000000000002</v>
+      </c>
+      <c r="L100" s="1">
+        <v>17.568999999999999</v>
+      </c>
+      <c r="M100" s="1">
+        <f t="shared" si="4"/>
+        <v>0.12299999999999756</v>
+      </c>
+      <c r="P100" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00</v>
       </c>
     </row>
-    <row r="101" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="8">
+    <row r="101" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="18">
         <v>43198</v>
       </c>
-      <c r="B101" s="9">
-        <v>1</v>
-      </c>
-      <c r="C101" s="9">
-        <v>1</v>
-      </c>
-      <c r="D101" s="9">
+      <c r="B101" s="5">
+        <v>1</v>
+      </c>
+      <c r="C101" s="5">
+        <v>1</v>
+      </c>
+      <c r="D101" s="5">
         <v>2</v>
       </c>
-      <c r="E101" s="9" t="s">
+      <c r="E101" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F101" s="9">
+      <c r="F101" s="5">
         <v>25</v>
       </c>
-      <c r="G101" s="9">
+      <c r="G101" s="5">
         <v>29</v>
       </c>
-      <c r="H101" s="10">
-        <v>1</v>
-      </c>
-      <c r="J101" s="10"/>
-      <c r="P101" s="15" t="str">
+      <c r="H101" s="6">
+        <v>1</v>
+      </c>
+      <c r="I101" s="20">
+        <v>28</v>
+      </c>
+      <c r="J101" s="20">
+        <v>25.2</v>
+      </c>
+      <c r="K101" s="5">
+        <v>17.178999999999998</v>
+      </c>
+      <c r="L101" s="5">
+        <v>17.32</v>
+      </c>
+      <c r="M101" s="5">
+        <f t="shared" si="4"/>
+        <v>0.14100000000000179</v>
+      </c>
+      <c r="P101" s="19" t="str">
         <f t="shared" si="3"/>
         <v>00</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="P1">
-    <cfRule type="dataBar" priority="13">
+    <cfRule type="dataBar" priority="24">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5465,7 +6200,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1">
-    <cfRule type="dataBar" priority="12">
+    <cfRule type="dataBar" priority="23">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5479,7 +6214,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1">
-    <cfRule type="dataBar" priority="11">
+    <cfRule type="dataBar" priority="22">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5493,7 +6228,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P1">
-    <cfRule type="dataBar" priority="10">
+    <cfRule type="dataBar" priority="21">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5507,7 +6242,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1">
-    <cfRule type="dataBar" priority="9">
+    <cfRule type="dataBar" priority="20">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5521,7 +6256,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P1">
-    <cfRule type="dataBar" priority="8">
+    <cfRule type="dataBar" priority="19">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5535,7 +6270,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K26">
-    <cfRule type="dataBar" priority="7">
+    <cfRule type="dataBar" priority="18">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5549,7 +6284,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:M26">
-    <cfRule type="dataBar" priority="5">
+    <cfRule type="dataBar" priority="16">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5563,7 +6298,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M26">
-    <cfRule type="dataBar" priority="4">
+    <cfRule type="dataBar" priority="15">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5576,8 +6311,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K27:K51">
-    <cfRule type="dataBar" priority="3">
+  <conditionalFormatting sqref="K27:K51 K53:K62">
+    <cfRule type="dataBar" priority="14">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5591,7 +6326,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L27:M51">
-    <cfRule type="dataBar" priority="2">
+    <cfRule type="dataBar" priority="13">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5605,6 +6340,160 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M27:M51">
+    <cfRule type="dataBar" priority="12">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{D1162CA9-164E-FC4C-B92D-5A5F8B4A401E}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K52">
+    <cfRule type="dataBar" priority="11">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{C9E85B1D-C158-9B46-9978-C8BBAAA057E8}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K63">
+    <cfRule type="dataBar" priority="10">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{D099768B-742F-F34D-A9CA-4CF2A1755558}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K1:K76 K102:K1048576">
+    <cfRule type="dataBar" priority="9">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{FB8F6B1B-DAC8-754C-BD9D-4EAC3B2EECD8}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L1:L76 L102:L1048576">
+    <cfRule type="dataBar" priority="8">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFB628"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{2EA429C5-A3E5-5140-AF59-75ED7E71812C}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M1:M76 M102:M1048576">
+    <cfRule type="dataBar" priority="7">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{EE24540D-BBEC-F44A-8B00-A901493F197E}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K78:K87">
+    <cfRule type="dataBar" priority="6">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{50E1FB89-B65C-0649-92DB-F8B1C7BF26F7}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K77">
+    <cfRule type="dataBar" priority="5">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{38688A9E-D790-FB4A-ABF4-812DD4B46A79}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K88">
+    <cfRule type="dataBar" priority="4">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{3535575B-AA76-5F47-ACC2-E76849D0D705}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K77:K101">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{279644BD-FDFB-5545-AB5C-A95D356E10C7}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L77:L101">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFB628"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{5292CBD9-01A4-AA49-A35E-492E779C3E4D}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M77:M101">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="min"/>
@@ -5613,7 +6502,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{D1162CA9-164E-FC4C-B92D-5A5F8B4A401E}</x14:id>
+          <x14:id>{80FE69A2-9826-1448-9121-AB5D1B879F95}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -5739,7 +6628,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>K27:K51</xm:sqref>
+          <xm:sqref>K27:K51 K53:K62</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{B6862059-F0B4-5144-8981-9036CA958C9D}">
@@ -5767,6 +6656,149 @@
           </x14:cfRule>
           <xm:sqref>M27:M51</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{C9E85B1D-C158-9B46-9978-C8BBAAA057E8}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>K52</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{D099768B-742F-F34D-A9CA-4CF2A1755558}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>K63</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{FB8F6B1B-DAC8-754C-BD9D-4EAC3B2EECD8}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>K1:K76 K102:K1048576</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{2EA429C5-A3E5-5140-AF59-75ED7E71812C}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFFB628"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>L1:L76 L102:L1048576</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{EE24540D-BBEC-F44A-8B00-A901493F197E}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>M1:M76 M102:M1048576</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{50E1FB89-B65C-0649-92DB-F8B1C7BF26F7}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>K78:K87</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{38688A9E-D790-FB4A-ABF4-812DD4B46A79}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>K77</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{3535575B-AA76-5F47-ACC2-E76849D0D705}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>K88</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{279644BD-FDFB-5545-AB5C-A95D356E10C7}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>K77:K101</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{5292CBD9-01A4-AA49-A35E-492E779C3E4D}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFFB628"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>L77:L101</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{80FE69A2-9826-1448-9121-AB5D1B879F95}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>M77:M101</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
entered data for 6/5/2017
</commit_message>
<xml_diff>
--- a/data/curve_data/ldeli_tinc_integrate.xlsx
+++ b/data/curve_data/ldeli_tinc_integrate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fontikar/Dropbox/Ldeli_inc_metabTelo/data/curve_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{156BEBCE-E04D-0244-A9CE-425A86F7B807}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB89232A-88D0-0B40-93C0-EB87A7277444}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="8320" windowWidth="25600" windowHeight="6640" xr2:uid="{84C113A7-A3A6-0745-8C21-C9F341A27D93}"/>
+    <workbookView xWindow="-60" yWindow="460" windowWidth="25600" windowHeight="14500" xr2:uid="{84C113A7-A3A6-0745-8C21-C9F341A27D93}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4589" uniqueCount="1392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4597" uniqueCount="1394">
   <si>
     <t>date</t>
   </si>
@@ -4201,6 +4201,12 @@
   </si>
   <si>
     <t> 9.755e-4</t>
+  </si>
+  <si>
+    <t>KO</t>
+  </si>
+  <si>
+    <t>T1S2NP</t>
   </si>
 </sst>
 </file>
@@ -4725,10 +4731,10 @@
   <dimension ref="A1:Z1301"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B650" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B694" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U652" sqref="U652"/>
+      <selection pane="bottomRight" activeCell="S706" sqref="S706"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -45970,6 +45976,9 @@
       <c r="S602" s="10" t="s">
         <v>49</v>
       </c>
+      <c r="T602" s="10">
+        <v>1</v>
+      </c>
       <c r="U602" s="10" t="s">
         <v>139</v>
       </c>
@@ -46034,6 +46043,9 @@
       <c r="S603" s="10" t="s">
         <v>50</v>
       </c>
+      <c r="T603" s="10">
+        <v>0</v>
+      </c>
       <c r="U603" s="1" t="s">
         <v>1303</v>
       </c>
@@ -46098,6 +46110,9 @@
       <c r="S604" s="10" t="s">
         <v>51</v>
       </c>
+      <c r="T604" s="10">
+        <v>1</v>
+      </c>
       <c r="U604" s="1" t="s">
         <v>1306</v>
       </c>
@@ -46162,6 +46177,9 @@
       <c r="S605" s="10" t="s">
         <v>52</v>
       </c>
+      <c r="T605" s="10">
+        <v>0</v>
+      </c>
       <c r="U605" s="1" t="s">
         <v>1309</v>
       </c>
@@ -46226,6 +46244,9 @@
       <c r="S606" s="10" t="s">
         <v>53</v>
       </c>
+      <c r="T606" s="10">
+        <v>1</v>
+      </c>
       <c r="U606" s="1" t="s">
         <v>1032</v>
       </c>
@@ -46290,6 +46311,9 @@
       <c r="S607" s="10" t="s">
         <v>54</v>
       </c>
+      <c r="T607" s="10">
+        <v>0</v>
+      </c>
       <c r="U607" s="1" t="s">
         <v>1314</v>
       </c>
@@ -46354,6 +46378,9 @@
       <c r="S608" s="10" t="s">
         <v>55</v>
       </c>
+      <c r="T608" s="10">
+        <v>0</v>
+      </c>
       <c r="U608" s="10" t="s">
         <v>139</v>
       </c>
@@ -46418,6 +46445,9 @@
       <c r="S609" s="10" t="s">
         <v>56</v>
       </c>
+      <c r="T609" s="10">
+        <v>1</v>
+      </c>
       <c r="U609" s="1" t="s">
         <v>1319</v>
       </c>
@@ -46482,6 +46512,9 @@
       <c r="S610" s="10" t="s">
         <v>57</v>
       </c>
+      <c r="T610" s="10">
+        <v>0</v>
+      </c>
       <c r="U610" s="1" t="s">
         <v>1322</v>
       </c>
@@ -46546,6 +46579,9 @@
       <c r="S611" s="10" t="s">
         <v>58</v>
       </c>
+      <c r="T611" s="10">
+        <v>0</v>
+      </c>
       <c r="U611" s="1" t="s">
         <v>1325</v>
       </c>
@@ -46610,6 +46646,9 @@
       <c r="S612" s="10" t="s">
         <v>59</v>
       </c>
+      <c r="T612" s="10">
+        <v>0</v>
+      </c>
       <c r="U612" s="1" t="s">
         <v>1331</v>
       </c>
@@ -46674,6 +46713,9 @@
       <c r="S613" s="10" t="s">
         <v>60</v>
       </c>
+      <c r="T613" s="10">
+        <v>0</v>
+      </c>
       <c r="U613" s="1" t="s">
         <v>1328</v>
       </c>
@@ -46738,6 +46780,9 @@
       <c r="S614" s="10" t="s">
         <v>61</v>
       </c>
+      <c r="T614" s="10">
+        <v>0</v>
+      </c>
       <c r="U614" s="1" t="s">
         <v>1333</v>
       </c>
@@ -46802,6 +46847,9 @@
       <c r="S615" s="10" t="s">
         <v>62</v>
       </c>
+      <c r="T615" s="10">
+        <v>0</v>
+      </c>
       <c r="U615" s="10" t="s">
         <v>139</v>
       </c>
@@ -46866,6 +46914,9 @@
       <c r="S616" s="10" t="s">
         <v>63</v>
       </c>
+      <c r="T616" s="10">
+        <v>1</v>
+      </c>
       <c r="U616" s="1" t="s">
         <v>1336</v>
       </c>
@@ -46930,6 +46981,9 @@
       <c r="S617" s="10" t="s">
         <v>64</v>
       </c>
+      <c r="T617" s="10">
+        <v>0</v>
+      </c>
       <c r="U617" s="1" t="s">
         <v>1337</v>
       </c>
@@ -46994,6 +47048,9 @@
       <c r="S618" s="10" t="s">
         <v>65</v>
       </c>
+      <c r="T618" s="10">
+        <v>0</v>
+      </c>
       <c r="U618" s="1" t="s">
         <v>1338</v>
       </c>
@@ -47058,6 +47115,9 @@
       <c r="S619" s="10" t="s">
         <v>66</v>
       </c>
+      <c r="T619" s="10">
+        <v>0</v>
+      </c>
       <c r="U619" s="1" t="s">
         <v>1340</v>
       </c>
@@ -47122,6 +47182,9 @@
       <c r="S620" s="10" t="s">
         <v>67</v>
       </c>
+      <c r="T620" s="10">
+        <v>1</v>
+      </c>
       <c r="U620" s="1" t="s">
         <v>1343</v>
       </c>
@@ -47186,6 +47249,9 @@
       <c r="S621" s="10" t="s">
         <v>68</v>
       </c>
+      <c r="T621" s="10">
+        <v>0</v>
+      </c>
       <c r="U621" s="1" t="s">
         <v>1340</v>
       </c>
@@ -47250,6 +47316,9 @@
       <c r="S622" s="10" t="s">
         <v>69</v>
       </c>
+      <c r="T622" s="10">
+        <v>0</v>
+      </c>
       <c r="U622" s="1" t="s">
         <v>1100</v>
       </c>
@@ -47314,6 +47383,9 @@
       <c r="S623" s="10" t="s">
         <v>72</v>
       </c>
+      <c r="T623" s="10">
+        <v>0</v>
+      </c>
       <c r="U623" s="10" t="s">
         <v>139</v>
       </c>
@@ -47378,6 +47450,9 @@
       <c r="S624" s="10" t="s">
         <v>71</v>
       </c>
+      <c r="T624" s="10">
+        <v>0</v>
+      </c>
       <c r="U624" s="10" t="s">
         <v>139</v>
       </c>
@@ -47442,6 +47517,9 @@
       <c r="S625" s="10" t="s">
         <v>70</v>
       </c>
+      <c r="T625" s="10">
+        <v>1</v>
+      </c>
       <c r="U625" s="1" t="s">
         <v>1348</v>
       </c>
@@ -47506,6 +47584,9 @@
       <c r="S626" s="18" t="s">
         <v>73</v>
       </c>
+      <c r="T626" s="18">
+        <v>0</v>
+      </c>
       <c r="U626" s="18" t="s">
         <v>139</v>
       </c>
@@ -47573,6 +47654,9 @@
       <c r="S627" s="10" t="s">
         <v>49</v>
       </c>
+      <c r="T627" s="10">
+        <v>1</v>
+      </c>
       <c r="U627" s="1" t="s">
         <v>1349</v>
       </c>
@@ -47637,6 +47721,9 @@
       <c r="S628" s="10" t="s">
         <v>50</v>
       </c>
+      <c r="T628" s="10">
+        <v>0</v>
+      </c>
       <c r="U628" s="10" t="s">
         <v>139</v>
       </c>
@@ -47701,6 +47788,9 @@
       <c r="S629" s="10" t="s">
         <v>51</v>
       </c>
+      <c r="T629" s="10">
+        <v>1</v>
+      </c>
       <c r="U629" s="1" t="s">
         <v>139</v>
       </c>
@@ -47765,6 +47855,9 @@
       <c r="S630" s="10" t="s">
         <v>52</v>
       </c>
+      <c r="T630" s="10">
+        <v>0</v>
+      </c>
       <c r="U630" s="10" t="s">
         <v>139</v>
       </c>
@@ -47829,6 +47922,9 @@
       <c r="S631" s="10" t="s">
         <v>53</v>
       </c>
+      <c r="T631" s="10">
+        <v>1</v>
+      </c>
       <c r="U631" s="10" t="s">
         <v>139</v>
       </c>
@@ -47893,6 +47989,9 @@
       <c r="S632" s="10" t="s">
         <v>54</v>
       </c>
+      <c r="T632" s="10">
+        <v>0</v>
+      </c>
       <c r="U632" s="10" t="s">
         <v>139</v>
       </c>
@@ -47957,6 +48056,9 @@
       <c r="S633" s="10" t="s">
         <v>55</v>
       </c>
+      <c r="T633" s="10">
+        <v>0</v>
+      </c>
       <c r="U633" s="1" t="s">
         <v>1359</v>
       </c>
@@ -48021,6 +48123,9 @@
       <c r="S634" s="10" t="s">
         <v>56</v>
       </c>
+      <c r="T634" s="10">
+        <v>1</v>
+      </c>
       <c r="U634" s="1" t="s">
         <v>139</v>
       </c>
@@ -48085,6 +48190,9 @@
       <c r="S635" s="10" t="s">
         <v>57</v>
       </c>
+      <c r="T635" s="10">
+        <v>0</v>
+      </c>
       <c r="U635" s="1" t="s">
         <v>1362</v>
       </c>
@@ -48149,6 +48257,9 @@
       <c r="S636" s="10" t="s">
         <v>58</v>
       </c>
+      <c r="T636" s="10">
+        <v>0</v>
+      </c>
       <c r="U636" s="1" t="s">
         <v>1365</v>
       </c>
@@ -48213,6 +48324,9 @@
       <c r="S637" s="10" t="s">
         <v>59</v>
       </c>
+      <c r="T637" s="10">
+        <v>0</v>
+      </c>
       <c r="U637" s="10" t="s">
         <v>139</v>
       </c>
@@ -48277,6 +48391,9 @@
       <c r="S638" s="10" t="s">
         <v>60</v>
       </c>
+      <c r="T638" s="10">
+        <v>0</v>
+      </c>
       <c r="U638" s="10" t="s">
         <v>139</v>
       </c>
@@ -48341,6 +48458,9 @@
       <c r="S639" s="10" t="s">
         <v>61</v>
       </c>
+      <c r="T639" s="10">
+        <v>0</v>
+      </c>
       <c r="U639" s="10" t="s">
         <v>139</v>
       </c>
@@ -48405,6 +48525,9 @@
       <c r="S640" s="10" t="s">
         <v>62</v>
       </c>
+      <c r="T640" s="10">
+        <v>0</v>
+      </c>
       <c r="U640" s="1" t="s">
         <v>1370</v>
       </c>
@@ -48415,7 +48538,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="641" spans="1:23" ht="21" x14ac:dyDescent="0.25">
+    <row r="641" spans="1:24" ht="21" x14ac:dyDescent="0.25">
       <c r="A641" s="9">
         <v>43225</v>
       </c>
@@ -48469,6 +48592,9 @@
       <c r="S641" s="10" t="s">
         <v>63</v>
       </c>
+      <c r="T641" s="10">
+        <v>1</v>
+      </c>
       <c r="U641" s="10" t="s">
         <v>139</v>
       </c>
@@ -48479,7 +48605,7 @@
         <v>1374</v>
       </c>
     </row>
-    <row r="642" spans="1:23" ht="21" x14ac:dyDescent="0.25">
+    <row r="642" spans="1:24" ht="21" x14ac:dyDescent="0.25">
       <c r="A642" s="9">
         <v>43225</v>
       </c>
@@ -48533,6 +48659,9 @@
       <c r="S642" s="10" t="s">
         <v>64</v>
       </c>
+      <c r="T642" s="10">
+        <v>0</v>
+      </c>
       <c r="U642" s="1" t="s">
         <v>1375</v>
       </c>
@@ -48543,7 +48672,7 @@
         <v>1377</v>
       </c>
     </row>
-    <row r="643" spans="1:23" ht="21" x14ac:dyDescent="0.25">
+    <row r="643" spans="1:24" ht="21" x14ac:dyDescent="0.25">
       <c r="A643" s="9">
         <v>43225</v>
       </c>
@@ -48597,6 +48726,9 @@
       <c r="S643" s="10" t="s">
         <v>65</v>
       </c>
+      <c r="T643" s="10">
+        <v>0</v>
+      </c>
       <c r="U643" s="10" t="s">
         <v>139</v>
       </c>
@@ -48607,7 +48739,7 @@
         <v>1379</v>
       </c>
     </row>
-    <row r="644" spans="1:23" ht="21" x14ac:dyDescent="0.25">
+    <row r="644" spans="1:24" ht="21" x14ac:dyDescent="0.25">
       <c r="A644" s="9">
         <v>43225</v>
       </c>
@@ -48661,6 +48793,9 @@
       <c r="S644" s="10" t="s">
         <v>66</v>
       </c>
+      <c r="T644" s="10">
+        <v>0</v>
+      </c>
       <c r="U644" s="10" t="s">
         <v>139</v>
       </c>
@@ -48671,7 +48806,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="645" spans="1:23" ht="21" x14ac:dyDescent="0.25">
+    <row r="645" spans="1:24" ht="21" x14ac:dyDescent="0.25">
       <c r="A645" s="9">
         <v>43225</v>
       </c>
@@ -48725,6 +48860,9 @@
       <c r="S645" s="10" t="s">
         <v>67</v>
       </c>
+      <c r="T645" s="10">
+        <v>1</v>
+      </c>
       <c r="U645" s="1" t="s">
         <v>1381</v>
       </c>
@@ -48735,7 +48873,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="646" spans="1:23" ht="21" x14ac:dyDescent="0.25">
+    <row r="646" spans="1:24" ht="21" x14ac:dyDescent="0.25">
       <c r="A646" s="9">
         <v>43225</v>
       </c>
@@ -48789,6 +48927,9 @@
       <c r="S646" s="10" t="s">
         <v>68</v>
       </c>
+      <c r="T646" s="10">
+        <v>0</v>
+      </c>
       <c r="U646" s="10" t="s">
         <v>139</v>
       </c>
@@ -48799,7 +48940,7 @@
         <v>1384</v>
       </c>
     </row>
-    <row r="647" spans="1:23" ht="21" x14ac:dyDescent="0.25">
+    <row r="647" spans="1:24" ht="21" x14ac:dyDescent="0.25">
       <c r="A647" s="9">
         <v>43225</v>
       </c>
@@ -48853,6 +48994,9 @@
       <c r="S647" s="10" t="s">
         <v>69</v>
       </c>
+      <c r="T647" s="10">
+        <v>0</v>
+      </c>
       <c r="U647" s="10" t="s">
         <v>139</v>
       </c>
@@ -48863,7 +49007,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="648" spans="1:23" ht="21" x14ac:dyDescent="0.25">
+    <row r="648" spans="1:24" ht="21" x14ac:dyDescent="0.25">
       <c r="A648" s="9">
         <v>43225</v>
       </c>
@@ -48917,6 +49061,9 @@
       <c r="S648" s="10" t="s">
         <v>72</v>
       </c>
+      <c r="T648" s="10">
+        <v>0</v>
+      </c>
       <c r="U648" s="10" t="s">
         <v>139</v>
       </c>
@@ -48927,7 +49074,7 @@
         <v>1386</v>
       </c>
     </row>
-    <row r="649" spans="1:23" ht="21" x14ac:dyDescent="0.25">
+    <row r="649" spans="1:24" ht="21" x14ac:dyDescent="0.25">
       <c r="A649" s="9">
         <v>43225</v>
       </c>
@@ -48981,6 +49128,9 @@
       <c r="S649" s="10" t="s">
         <v>71</v>
       </c>
+      <c r="T649" s="10">
+        <v>0</v>
+      </c>
       <c r="U649" s="1" t="s">
         <v>1387</v>
       </c>
@@ -48991,7 +49141,7 @@
         <v>1388</v>
       </c>
     </row>
-    <row r="650" spans="1:23" ht="21" x14ac:dyDescent="0.25">
+    <row r="650" spans="1:24" ht="21" x14ac:dyDescent="0.25">
       <c r="A650" s="9">
         <v>43225</v>
       </c>
@@ -49045,6 +49195,9 @@
       <c r="S650" s="10" t="s">
         <v>70</v>
       </c>
+      <c r="T650" s="10">
+        <v>1</v>
+      </c>
       <c r="U650" s="1" t="s">
         <v>1389</v>
       </c>
@@ -49055,7 +49208,7 @@
         <v>1.2149999999999999E-3</v>
       </c>
     </row>
-    <row r="651" spans="1:23" s="18" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="651" spans="1:24" s="18" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A651" s="17">
         <v>43225</v>
       </c>
@@ -49109,6 +49262,9 @@
       <c r="S651" s="18" t="s">
         <v>73</v>
       </c>
+      <c r="T651" s="18">
+        <v>0</v>
+      </c>
       <c r="U651" s="18" t="s">
         <v>139</v>
       </c>
@@ -49119,7 +49275,7 @@
         <v>1391</v>
       </c>
     </row>
-    <row r="652" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="652" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A652" s="9">
         <v>43226</v>
       </c>
@@ -49173,8 +49329,11 @@
       <c r="S652" s="10" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="653" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="T652" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="653" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A653" s="9">
         <v>43226</v>
       </c>
@@ -49228,8 +49387,11 @@
       <c r="S653" s="10" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="654" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="T653" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="654" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A654" s="9">
         <v>43226</v>
       </c>
@@ -49283,8 +49445,11 @@
       <c r="S654" s="10" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="655" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="T654" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="655" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A655" s="9">
         <v>43226</v>
       </c>
@@ -49338,8 +49503,11 @@
       <c r="S655" s="10" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="656" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="T655" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="656" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A656" s="9">
         <v>43226</v>
       </c>
@@ -49393,8 +49561,14 @@
       <c r="S656" s="10" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="657" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T656" s="10">
+        <v>0</v>
+      </c>
+      <c r="X656" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="657" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A657" s="9">
         <v>43226</v>
       </c>
@@ -49448,8 +49622,11 @@
       <c r="S657" s="10" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="658" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T657" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="658" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A658" s="9">
         <v>43226</v>
       </c>
@@ -49503,8 +49680,11 @@
       <c r="S658" s="10" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="659" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T658" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="659" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A659" s="9">
         <v>43226</v>
       </c>
@@ -49558,8 +49738,11 @@
       <c r="S659" s="10" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="660" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T659" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="660" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A660" s="9">
         <v>43226</v>
       </c>
@@ -49613,8 +49796,14 @@
       <c r="S660" s="10" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="661" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T660" s="10">
+        <v>0</v>
+      </c>
+      <c r="X660" s="10" t="s">
+        <v>1393</v>
+      </c>
+    </row>
+    <row r="661" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A661" s="9">
         <v>43226</v>
       </c>
@@ -49668,8 +49857,11 @@
       <c r="S661" s="10" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="662" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T661" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="662" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A662" s="9">
         <v>43226</v>
       </c>
@@ -49723,63 +49915,69 @@
       <c r="S662" s="10" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="663" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A663" s="9">
+      <c r="T662" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="663" spans="1:24" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A663" s="17">
         <v>43226</v>
       </c>
-      <c r="B663" s="10">
+      <c r="B663" s="18">
         <v>4</v>
       </c>
-      <c r="C663" s="10">
-        <v>1</v>
-      </c>
-      <c r="D663" s="10">
-        <v>1</v>
-      </c>
-      <c r="E663" s="10" t="s">
+      <c r="C663" s="18">
+        <v>1</v>
+      </c>
+      <c r="D663" s="18">
+        <v>1</v>
+      </c>
+      <c r="E663" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="F663" s="10">
+      <c r="F663" s="18">
         <v>12</v>
       </c>
-      <c r="G663" s="10">
+      <c r="G663" s="18">
         <v>29</v>
       </c>
-      <c r="H663" s="10">
-        <v>1</v>
-      </c>
-      <c r="I663" s="10">
+      <c r="H663" s="18">
+        <v>1</v>
+      </c>
+      <c r="I663" s="18">
         <v>32</v>
       </c>
-      <c r="J663" s="10">
+      <c r="J663" s="18">
         <v>20</v>
       </c>
-      <c r="K663" s="10">
+      <c r="K663" s="18">
         <v>17.096</v>
       </c>
-      <c r="L663" s="10">
+      <c r="L663" s="18">
         <v>17.332000000000001</v>
       </c>
-      <c r="M663" s="10">
+      <c r="M663" s="18">
         <f t="shared" si="27"/>
         <v>0.23600000000000065</v>
       </c>
-      <c r="O663" s="12">
+      <c r="O663" s="20">
         <v>0.391666666666666</v>
       </c>
-      <c r="P663" s="12">
+      <c r="P663" s="20">
         <v>0.47499999999999898</v>
       </c>
-      <c r="Q663" s="10" t="str">
+      <c r="Q663" s="18" t="str">
         <f t="shared" si="26"/>
         <v>120</v>
       </c>
-      <c r="S663" s="10" t="s">
+      <c r="S663" s="18" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="664" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T663" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="664" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A664" s="9">
         <v>43226</v>
       </c>
@@ -49833,8 +50031,11 @@
       <c r="S664" s="10" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="665" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T664" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="665" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A665" s="9">
         <v>43226</v>
       </c>
@@ -49888,8 +50089,11 @@
       <c r="S665" s="10" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="666" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T665" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="666" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A666" s="9">
         <v>43226</v>
       </c>
@@ -49943,8 +50147,11 @@
       <c r="S666" s="10" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="667" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T666" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="667" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A667" s="9">
         <v>43226</v>
       </c>
@@ -49998,8 +50205,11 @@
       <c r="S667" s="10" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="668" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T667" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="668" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A668" s="9">
         <v>43226</v>
       </c>
@@ -50053,8 +50263,11 @@
       <c r="S668" s="10" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="669" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T668" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="669" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A669" s="9">
         <v>43226</v>
       </c>
@@ -50108,8 +50321,11 @@
       <c r="S669" s="10" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="670" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T669" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="670" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A670" s="9">
         <v>43226</v>
       </c>
@@ -50163,8 +50379,11 @@
       <c r="S670" s="10" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="671" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T670" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="671" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A671" s="9">
         <v>43226</v>
       </c>
@@ -50218,8 +50437,11 @@
       <c r="S671" s="10" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="672" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T671" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="672" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A672" s="9">
         <v>43226</v>
       </c>
@@ -50273,8 +50495,14 @@
       <c r="S672" s="10" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="673" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T672" s="10">
+        <v>0</v>
+      </c>
+      <c r="X672" s="10" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="673" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A673" s="9">
         <v>43226</v>
       </c>
@@ -50328,8 +50556,11 @@
       <c r="S673" s="10" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="674" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T673" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="674" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A674" s="9">
         <v>43226</v>
       </c>
@@ -50383,8 +50614,11 @@
       <c r="S674" s="10" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="675" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T674" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="675" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A675" s="9">
         <v>43226</v>
       </c>
@@ -50438,63 +50672,72 @@
       <c r="S675" s="10" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="676" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A676" s="9">
+      <c r="T675" s="10">
+        <v>0</v>
+      </c>
+      <c r="X675" s="10" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="676" spans="1:24" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A676" s="17">
         <v>43226</v>
       </c>
-      <c r="B676" s="10">
+      <c r="B676" s="18">
         <v>4</v>
       </c>
-      <c r="C676" s="10">
-        <v>1</v>
-      </c>
-      <c r="D676" s="10">
-        <v>2</v>
-      </c>
-      <c r="E676" s="10" t="s">
+      <c r="C676" s="18">
+        <v>1</v>
+      </c>
+      <c r="D676" s="18">
+        <v>2</v>
+      </c>
+      <c r="E676" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F676" s="10">
+      <c r="F676" s="18">
         <v>25</v>
       </c>
-      <c r="G676" s="10">
+      <c r="G676" s="18">
         <v>23</v>
       </c>
-      <c r="H676" s="10">
-        <v>1</v>
-      </c>
-      <c r="I676" s="10">
+      <c r="H676" s="18">
+        <v>1</v>
+      </c>
+      <c r="I676" s="18">
         <v>28</v>
       </c>
-      <c r="J676" s="10">
+      <c r="J676" s="18">
         <v>19.399999999999999</v>
       </c>
-      <c r="K676" s="10">
+      <c r="K676" s="18">
         <v>17.297999999999998</v>
       </c>
-      <c r="L676" s="10">
+      <c r="L676" s="18">
         <v>17.518999999999998</v>
       </c>
-      <c r="M676" s="10">
+      <c r="M676" s="18">
         <f t="shared" si="27"/>
         <v>0.22100000000000009</v>
       </c>
-      <c r="O676" s="12">
+      <c r="O676" s="20">
         <v>0.41319444444444398</v>
       </c>
-      <c r="P676" s="12">
+      <c r="P676" s="20">
         <v>0.49652777777777801</v>
       </c>
-      <c r="Q676" s="10" t="str">
+      <c r="Q676" s="18" t="str">
         <f t="shared" si="28"/>
         <v>120</v>
       </c>
-      <c r="S676" s="10" t="s">
+      <c r="S676" s="18" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="677" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T676" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="677" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A677" s="9">
         <v>43226</v>
       </c>
@@ -50548,8 +50791,11 @@
       <c r="S677" s="10" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="678" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T677" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="678" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A678" s="9">
         <v>43226</v>
       </c>
@@ -50603,8 +50849,11 @@
       <c r="S678" s="10" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="679" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T678" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="679" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A679" s="9">
         <v>43226</v>
       </c>
@@ -50658,8 +50907,11 @@
       <c r="S679" s="10" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="680" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T679" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="680" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A680" s="9">
         <v>43226</v>
       </c>
@@ -50713,8 +50965,11 @@
       <c r="S680" s="10" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="681" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T680" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="681" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A681" s="9">
         <v>43226</v>
       </c>
@@ -50768,8 +51023,14 @@
       <c r="S681" s="10" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="682" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T681" s="10">
+        <v>0</v>
+      </c>
+      <c r="X681" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="682" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A682" s="9">
         <v>43226</v>
       </c>
@@ -50823,8 +51084,11 @@
       <c r="S682" s="10" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="683" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T682" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="683" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A683" s="9">
         <v>43226</v>
       </c>
@@ -50878,8 +51142,11 @@
       <c r="S683" s="10" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="684" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T683" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="684" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A684" s="9">
         <v>43226</v>
       </c>
@@ -50933,8 +51200,11 @@
       <c r="S684" s="10" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="685" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T684" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="685" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A685" s="9">
         <v>43226</v>
       </c>
@@ -50988,8 +51258,14 @@
       <c r="S685" s="10" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="686" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T685" s="10">
+        <v>0</v>
+      </c>
+      <c r="X685" s="10" t="s">
+        <v>1393</v>
+      </c>
+    </row>
+    <row r="686" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A686" s="9">
         <v>43226</v>
       </c>
@@ -51043,8 +51319,11 @@
       <c r="S686" s="10" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="687" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T686" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="687" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A687" s="9">
         <v>43226</v>
       </c>
@@ -51098,63 +51377,69 @@
       <c r="S687" s="10" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="688" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A688" s="9">
+      <c r="T687" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="688" spans="1:24" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A688" s="17">
         <v>43226</v>
       </c>
-      <c r="B688" s="10">
+      <c r="B688" s="18">
         <v>4</v>
       </c>
-      <c r="C688" s="10">
-        <v>1</v>
-      </c>
-      <c r="D688" s="10">
-        <v>1</v>
-      </c>
-      <c r="E688" s="10" t="s">
+      <c r="C688" s="18">
+        <v>1</v>
+      </c>
+      <c r="D688" s="18">
+        <v>1</v>
+      </c>
+      <c r="E688" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="F688" s="10">
+      <c r="F688" s="18">
         <v>12</v>
       </c>
-      <c r="G688" s="10">
+      <c r="G688" s="18">
         <v>29</v>
       </c>
-      <c r="H688" s="10">
-        <v>2</v>
-      </c>
-      <c r="I688" s="10">
+      <c r="H688" s="18">
+        <v>2</v>
+      </c>
+      <c r="I688" s="18">
         <v>24</v>
       </c>
-      <c r="J688" s="10">
+      <c r="J688" s="18">
         <v>20</v>
       </c>
-      <c r="K688" s="10">
+      <c r="K688" s="18">
         <v>17.096</v>
       </c>
-      <c r="L688" s="10">
+      <c r="L688" s="18">
         <v>17.332000000000001</v>
       </c>
-      <c r="M688" s="10">
+      <c r="M688" s="18">
         <f t="shared" si="29"/>
         <v>0.23600000000000065</v>
       </c>
-      <c r="O688" s="12">
+      <c r="O688" s="20">
         <v>0.51805555555555705</v>
       </c>
-      <c r="P688" s="12">
+      <c r="P688" s="20">
         <v>0.64305555555555705</v>
       </c>
-      <c r="Q688" s="10" t="str">
+      <c r="Q688" s="18" t="str">
         <f t="shared" si="28"/>
         <v>180</v>
       </c>
-      <c r="S688" s="10" t="s">
+      <c r="S688" s="18" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="689" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T688" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="689" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A689" s="9">
         <v>43226</v>
       </c>
@@ -51208,8 +51493,11 @@
       <c r="S689" s="10" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="690" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T689" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="690" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A690" s="9">
         <v>43226</v>
       </c>
@@ -51263,8 +51551,11 @@
       <c r="S690" s="10" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="691" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T690" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="691" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A691" s="9">
         <v>43226</v>
       </c>
@@ -51318,8 +51609,11 @@
       <c r="S691" s="10" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="692" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T691" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="692" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A692" s="9">
         <v>43226</v>
       </c>
@@ -51373,8 +51667,11 @@
       <c r="S692" s="10" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="693" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T692" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="693" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A693" s="9">
         <v>43226</v>
       </c>
@@ -51428,8 +51725,11 @@
       <c r="S693" s="10" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="694" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T693" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="694" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A694" s="9">
         <v>43226</v>
       </c>
@@ -51483,8 +51783,11 @@
       <c r="S694" s="10" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="695" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T694" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="695" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A695" s="9">
         <v>43226</v>
       </c>
@@ -51538,8 +51841,11 @@
       <c r="S695" s="10" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="696" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T695" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="696" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A696" s="9">
         <v>43226</v>
       </c>
@@ -51593,8 +51899,11 @@
       <c r="S696" s="10" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="697" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T696" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="697" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A697" s="9">
         <v>43226</v>
       </c>
@@ -51648,8 +51957,14 @@
       <c r="S697" s="10" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="698" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T697" s="10">
+        <v>0</v>
+      </c>
+      <c r="X697" s="10" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="698" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A698" s="9">
         <v>43226</v>
       </c>
@@ -51703,8 +52018,11 @@
       <c r="S698" s="10" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="699" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T698" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="699" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A699" s="9">
         <v>43226</v>
       </c>
@@ -51758,8 +52076,11 @@
       <c r="S699" s="10" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="700" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T699" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="700" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A700" s="9">
         <v>43226</v>
       </c>
@@ -51813,8 +52134,14 @@
       <c r="S700" s="10" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="701" spans="1:19" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="T700" s="10">
+        <v>0</v>
+      </c>
+      <c r="X700" s="10" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="701" spans="1:24" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A701" s="17">
         <v>43226</v>
       </c>
@@ -51839,26 +52166,26 @@
       <c r="H701" s="18">
         <v>2</v>
       </c>
-      <c r="I701" s="10">
+      <c r="I701" s="18">
         <v>32</v>
       </c>
-      <c r="J701" s="10">
+      <c r="J701" s="18">
         <v>19.399999999999999</v>
       </c>
-      <c r="K701" s="10">
+      <c r="K701" s="18">
         <v>17.297999999999998</v>
       </c>
-      <c r="L701" s="10">
+      <c r="L701" s="18">
         <v>17.518999999999998</v>
       </c>
-      <c r="M701" s="10">
+      <c r="M701" s="18">
         <f t="shared" si="29"/>
         <v>0.22100000000000009</v>
       </c>
-      <c r="O701" s="12">
+      <c r="O701" s="20">
         <v>0.54027777777777797</v>
       </c>
-      <c r="P701" s="12">
+      <c r="P701" s="20">
         <v>0.62361111111111101</v>
       </c>
       <c r="Q701" s="18" t="str">
@@ -51868,8 +52195,11 @@
       <c r="S701" s="18" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="702" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T701" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="702" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A702" s="9">
         <v>43227</v>
       </c>
@@ -51908,7 +52238,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="703" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="703" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A703" s="9">
         <v>43227</v>
       </c>
@@ -51941,7 +52271,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="704" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="704" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A704" s="9">
         <v>43227</v>
       </c>

</xml_diff>